<commit_message>
Q11 round3 -没问题，Q15 round3 边界值
</commit_message>
<xml_diff>
--- a/code/src/main/leetcode.xlsx
+++ b/code/src/main/leetcode.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CE911F-075A-194C-82F3-1972067486C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EE8E0B-5183-BA4B-BA4E-A2B861FF136F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="331">
   <si>
     <t>题号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1322,6 +1322,10 @@
   </si>
   <si>
     <t>数组和链表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>——</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1329,6 +1333,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="yyyy/m/d;@"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -1403,7 +1410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1450,12 +1457,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1466,23 +1497,34 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1769,43 +1811,45 @@
   <dimension ref="A1:K141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="106.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="24" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.83203125" style="24"/>
+    <col min="11" max="11" width="106.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29" customHeight="1">
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:11" ht="29" customHeight="1">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="17" t="s">
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="16" t="s">
         <v>329</v>
       </c>
       <c r="B2">
@@ -1814,1357 +1858,1452 @@
       <c r="C2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="17"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="16"/>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22">
+        <v>44074</v>
+      </c>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="17"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="16"/>
       <c r="B4">
         <v>283</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="17"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="16"/>
       <c r="B5">
         <v>70</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="17"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="16"/>
       <c r="B6">
         <v>15</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="22">
+        <v>44006</v>
+      </c>
+      <c r="F6" s="22">
+        <v>44042</v>
+      </c>
+      <c r="G6" s="22">
+        <v>44074</v>
+      </c>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="17"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="16"/>
       <c r="B7">
         <v>11</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="22">
+        <v>44006</v>
+      </c>
+      <c r="F7" s="22">
+        <v>44040</v>
+      </c>
+      <c r="G7" s="22">
+        <v>44074</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="17"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="16"/>
       <c r="B8">
         <v>206</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="17"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="16"/>
       <c r="B9">
         <v>24</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="17"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="16"/>
       <c r="B10">
         <v>141</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="17"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="16"/>
       <c r="B11">
         <v>142</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="17"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="16"/>
       <c r="B12">
         <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="17"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="16"/>
       <c r="B13">
         <v>20</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="17"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="16"/>
       <c r="B14">
         <v>155</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="17"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="16"/>
       <c r="B15">
         <v>84</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="17"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="16"/>
       <c r="B16">
         <v>239</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="17"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="16"/>
       <c r="B17">
         <v>641</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="17"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="16"/>
       <c r="B18">
         <v>42</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="17"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="16"/>
       <c r="B19">
         <v>26</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="17"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="16"/>
       <c r="B20">
         <v>189</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="17"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="16"/>
       <c r="B21">
         <v>21</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="17"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="16"/>
       <c r="B22">
         <v>88</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="17"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="16"/>
       <c r="B23">
         <v>66</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="16"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="17"/>
       <c r="B24">
         <v>242</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="18"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="14"/>
       <c r="B25">
         <v>94</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:10">
+    </row>
+    <row r="26" spans="1:11">
       <c r="B26">
         <v>40</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10">
+    </row>
+    <row r="27" spans="1:11">
       <c r="B27">
         <v>144</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10">
+    </row>
+    <row r="28" spans="1:11">
       <c r="B28">
         <v>590</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10">
+    </row>
+    <row r="29" spans="1:11">
       <c r="B29">
         <v>589</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10">
+    </row>
+    <row r="30" spans="1:11">
       <c r="B30">
         <v>429</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10">
+    </row>
+    <row r="31" spans="1:11">
       <c r="B31">
         <v>49</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:10">
+    </row>
+    <row r="32" spans="1:11">
       <c r="B32">
         <v>347</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="2:10">
+    </row>
+    <row r="33" spans="2:11">
       <c r="B33">
         <v>200</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="2:10">
+    </row>
+    <row r="34" spans="2:11">
       <c r="B34">
         <v>49</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="2:10">
+    </row>
+    <row r="35" spans="2:11">
       <c r="B35">
         <v>22</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="2:10">
+    </row>
+    <row r="36" spans="2:11">
       <c r="B36">
         <v>50</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="2:10">
+    </row>
+    <row r="37" spans="2:11">
       <c r="B37">
         <v>78</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="2:10">
+    </row>
+    <row r="38" spans="2:11">
       <c r="B38">
         <v>51</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-    </row>
-    <row r="39" spans="2:10">
+    </row>
+    <row r="39" spans="2:11">
       <c r="B39">
         <v>226</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-    </row>
-    <row r="40" spans="2:10">
+    </row>
+    <row r="40" spans="2:11">
       <c r="B40">
         <v>98</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-    </row>
-    <row r="41" spans="2:10">
+    </row>
+    <row r="41" spans="2:11">
       <c r="B41">
         <v>104</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="2:10">
+    </row>
+    <row r="42" spans="2:11">
       <c r="B42">
         <v>111</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="2"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="2:10">
+    </row>
+    <row r="43" spans="2:11">
       <c r="B43">
         <v>297</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="2:10">
+    </row>
+    <row r="44" spans="2:11">
       <c r="B44">
         <v>236</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="2"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="2:10">
+    </row>
+    <row r="45" spans="2:11">
       <c r="B45">
         <v>105</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="2"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="2:10">
+    </row>
+    <row r="46" spans="2:11">
       <c r="B46">
         <v>77</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="2"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="2:10">
+    </row>
+    <row r="47" spans="2:11">
       <c r="B47">
         <v>46</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="2:10">
+    </row>
+    <row r="48" spans="2:11">
       <c r="B48">
         <v>47</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="2"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-    </row>
-    <row r="49" spans="2:10">
+    </row>
+    <row r="49" spans="2:11">
       <c r="B49">
         <v>17</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="2"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-    </row>
-    <row r="50" spans="2:10">
+    </row>
+    <row r="50" spans="2:11">
       <c r="B50">
         <v>169</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="2"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-    </row>
-    <row r="51" spans="2:10">
+    </row>
+    <row r="51" spans="2:11">
       <c r="B51">
         <v>455</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="2"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-    </row>
-    <row r="52" spans="2:10">
+    </row>
+    <row r="52" spans="2:11">
       <c r="B52">
         <v>55</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="2"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-    </row>
-    <row r="53" spans="2:10">
+    </row>
+    <row r="53" spans="2:11">
       <c r="B53">
         <v>69</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="2"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
+      <c r="K53" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-    </row>
-    <row r="54" spans="2:10">
+    </row>
+    <row r="54" spans="2:11">
       <c r="B54">
         <v>367</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="2"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-    </row>
-    <row r="55" spans="2:10">
+    </row>
+    <row r="55" spans="2:11">
       <c r="B55">
         <v>102</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="2"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="22"/>
+      <c r="K55" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-    </row>
-    <row r="56" spans="2:10">
+    </row>
+    <row r="56" spans="2:11">
       <c r="B56">
         <v>529</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="2"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="22"/>
+      <c r="I56" s="22"/>
+      <c r="J56" s="22"/>
+      <c r="K56" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-    </row>
-    <row r="57" spans="2:10">
+    </row>
+    <row r="57" spans="2:11">
       <c r="B57">
         <v>126</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="2"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="22"/>
+      <c r="I57" s="22"/>
+      <c r="J57" s="22"/>
+      <c r="K57" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-    </row>
-    <row r="58" spans="2:10">
+    </row>
+    <row r="58" spans="2:11">
       <c r="B58">
         <v>127</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="2"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="22"/>
+      <c r="I58" s="22"/>
+      <c r="J58" s="22"/>
+      <c r="K58" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-    </row>
-    <row r="59" spans="2:10">
+    </row>
+    <row r="59" spans="2:11">
       <c r="B59">
         <v>515</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="2"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="22"/>
+      <c r="I59" s="22"/>
+      <c r="J59" s="22"/>
+      <c r="K59" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-    </row>
-    <row r="60" spans="2:10">
+    </row>
+    <row r="60" spans="2:11">
       <c r="B60">
         <v>433</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="2"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
+      <c r="K60" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-    </row>
-    <row r="61" spans="2:10">
+    </row>
+    <row r="61" spans="2:11">
       <c r="B61">
         <v>1122</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="2"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="22"/>
+      <c r="I61" s="22"/>
+      <c r="J61" s="22"/>
+      <c r="K61" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-    </row>
-    <row r="62" spans="2:10">
+    </row>
+    <row r="62" spans="2:11">
       <c r="B62">
         <v>56</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="2"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="22"/>
+      <c r="I62" s="22"/>
+      <c r="J62" s="22"/>
+      <c r="K62" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-    </row>
-    <row r="63" spans="2:10">
+    </row>
+    <row r="63" spans="2:11">
       <c r="B63">
         <v>493</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="2"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="22"/>
+      <c r="J63" s="22"/>
+      <c r="K63" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-    </row>
-    <row r="64" spans="2:10">
+    </row>
+    <row r="64" spans="2:11">
       <c r="B64">
         <v>860</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="2"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="22"/>
+      <c r="I64" s="22"/>
+      <c r="J64" s="22"/>
+      <c r="K64" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-    </row>
-    <row r="65" spans="2:10">
+    </row>
+    <row r="65" spans="2:11">
       <c r="B65">
         <v>874</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="2"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="22"/>
+      <c r="I65" s="22"/>
+      <c r="J65" s="22"/>
+      <c r="K65" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-    </row>
-    <row r="66" spans="2:10">
+    </row>
+    <row r="66" spans="2:11">
       <c r="B66">
         <v>45</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="2"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="22"/>
+      <c r="H66" s="22"/>
+      <c r="I66" s="22"/>
+      <c r="J66" s="22"/>
+      <c r="K66" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-    </row>
-    <row r="67" spans="2:10">
+    </row>
+    <row r="67" spans="2:11">
       <c r="B67">
         <v>33</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="2"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="22"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="22"/>
+      <c r="K67" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-    </row>
-    <row r="68" spans="2:10">
+    </row>
+    <row r="68" spans="2:11">
       <c r="B68">
         <v>74</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="2"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="22"/>
+      <c r="G68" s="22"/>
+      <c r="H68" s="22"/>
+      <c r="I68" s="22"/>
+      <c r="J68" s="22"/>
+      <c r="K68" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-    </row>
-    <row r="69" spans="2:10">
+    </row>
+    <row r="69" spans="2:11">
       <c r="B69">
         <v>153</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="2"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="22"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="22"/>
+      <c r="K69" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
-    </row>
-    <row r="70" spans="2:10">
+    </row>
+    <row r="70" spans="2:11">
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-    </row>
-    <row r="71" spans="2:10">
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+      <c r="H70" s="22"/>
+      <c r="I70" s="22"/>
+      <c r="J70" s="22"/>
+      <c r="K70" s="2"/>
+    </row>
+    <row r="71" spans="2:11">
       <c r="B71" s="8">
         <v>62</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="2"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
+      <c r="H71" s="22"/>
+      <c r="I71" s="22"/>
+      <c r="J71" s="22"/>
+      <c r="K71" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
-    </row>
-    <row r="72" spans="2:10">
+    </row>
+    <row r="72" spans="2:11">
       <c r="B72" s="8">
         <v>63</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" s="2"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
+      <c r="H72" s="22"/>
+      <c r="I72" s="22"/>
+      <c r="J72" s="22"/>
+      <c r="K72" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E72" s="2"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
-    </row>
-    <row r="73" spans="2:10">
+    </row>
+    <row r="73" spans="2:11">
       <c r="B73" s="8">
         <v>1143</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D73" s="2"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="22"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="22"/>
+      <c r="K73" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E73" s="2"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-    </row>
-    <row r="74" spans="2:10">
+    </row>
+    <row r="74" spans="2:11">
       <c r="B74" s="8">
         <v>70</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D74" s="2"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
+      <c r="I74" s="22"/>
+      <c r="J74" s="22"/>
+      <c r="K74" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="E74" s="2"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-    </row>
-    <row r="75" spans="2:10">
+    </row>
+    <row r="75" spans="2:11">
       <c r="B75" s="8">
         <v>120</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D75" s="2"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="22"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="22"/>
+      <c r="I75" s="22"/>
+      <c r="J75" s="22"/>
+      <c r="K75" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
-    </row>
-    <row r="76" spans="2:10">
+    </row>
+    <row r="76" spans="2:11">
       <c r="B76" s="8">
         <v>53</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D76" s="2"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="22"/>
+      <c r="G76" s="22"/>
+      <c r="H76" s="22"/>
+      <c r="I76" s="22"/>
+      <c r="J76" s="22"/>
+      <c r="K76" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
-    </row>
-    <row r="77" spans="2:10">
+    </row>
+    <row r="77" spans="2:11">
       <c r="B77" s="8">
         <v>152</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D77" s="2"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="22"/>
+      <c r="G77" s="22"/>
+      <c r="H77" s="22"/>
+      <c r="I77" s="22"/>
+      <c r="J77" s="22"/>
+      <c r="K77" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="2"/>
-      <c r="J77" s="2"/>
-    </row>
-    <row r="78" spans="2:10">
+    </row>
+    <row r="78" spans="2:11">
       <c r="B78" s="8">
         <v>322</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D78" s="2"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="22"/>
+      <c r="G78" s="22"/>
+      <c r="H78" s="22"/>
+      <c r="I78" s="22"/>
+      <c r="J78" s="22"/>
+      <c r="K78" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E78" s="2"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-    </row>
-    <row r="79" spans="2:10">
+    </row>
+    <row r="79" spans="2:11">
       <c r="B79" s="8">
         <v>518</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D79" s="2"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="22"/>
+      <c r="I79" s="22"/>
+      <c r="J79" s="22"/>
+      <c r="K79" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E79" s="2"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-    </row>
-    <row r="80" spans="2:10">
+    </row>
+    <row r="80" spans="2:11">
       <c r="B80" s="8">
         <v>198</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="D80" s="2"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="22"/>
+      <c r="H80" s="22"/>
+      <c r="I80" s="22"/>
+      <c r="J80" s="22"/>
+      <c r="K80" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E80" s="2"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
     </row>
     <row r="81" spans="2:11">
       <c r="B81" s="8">
@@ -3173,15 +3312,16 @@
       <c r="C81" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D81" s="2"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="22"/>
+      <c r="H81" s="22"/>
+      <c r="I81" s="22"/>
+      <c r="J81" s="22"/>
+      <c r="K81" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
-      <c r="J81" s="2"/>
     </row>
     <row r="82" spans="2:11">
       <c r="B82" s="8">
@@ -3190,15 +3330,16 @@
       <c r="C82" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D82" s="2"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
+      <c r="H82" s="22"/>
+      <c r="I82" s="22"/>
+      <c r="J82" s="22"/>
+      <c r="K82" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
     </row>
     <row r="83" spans="2:11">
       <c r="B83" s="8">
@@ -3207,15 +3348,16 @@
       <c r="C83" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D83" s="2"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="22"/>
+      <c r="H83" s="22"/>
+      <c r="I83" s="22"/>
+      <c r="J83" s="22"/>
+      <c r="K83" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
-      <c r="J83" s="2"/>
     </row>
     <row r="84" spans="2:11">
       <c r="B84" s="8">
@@ -3224,15 +3366,16 @@
       <c r="C84" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="D84" s="2"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="22"/>
+      <c r="G84" s="22"/>
+      <c r="H84" s="22"/>
+      <c r="I84" s="22"/>
+      <c r="J84" s="22"/>
+      <c r="K84" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
     </row>
     <row r="85" spans="2:11">
       <c r="B85" s="8">
@@ -3241,15 +3384,16 @@
       <c r="C85" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" s="2"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="22"/>
+      <c r="H85" s="22"/>
+      <c r="I85" s="22"/>
+      <c r="J85" s="22"/>
+      <c r="K85" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
     </row>
     <row r="86" spans="2:11">
       <c r="B86" s="8">
@@ -3258,15 +3402,16 @@
       <c r="C86" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D86" s="2"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
+      <c r="G86" s="22"/>
+      <c r="H86" s="22"/>
+      <c r="I86" s="22"/>
+      <c r="J86" s="22"/>
+      <c r="K86" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="2"/>
     </row>
     <row r="87" spans="2:11">
       <c r="B87" s="8">
@@ -3275,16 +3420,16 @@
       <c r="C87" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D87" s="2"/>
+      <c r="E87" s="22"/>
+      <c r="F87" s="22"/>
+      <c r="G87" s="22"/>
+      <c r="H87" s="22"/>
+      <c r="I87" s="22"/>
+      <c r="J87" s="22"/>
+      <c r="K87" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2"/>
-      <c r="K87" s="5"/>
     </row>
     <row r="88" spans="2:11">
       <c r="B88" s="8">
@@ -3293,15 +3438,16 @@
       <c r="C88" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="D88" s="2"/>
+      <c r="E88" s="22"/>
+      <c r="F88" s="22"/>
+      <c r="G88" s="22"/>
+      <c r="H88" s="22"/>
+      <c r="I88" s="22"/>
+      <c r="J88" s="22"/>
+      <c r="K88" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
-      <c r="J88" s="2"/>
     </row>
     <row r="89" spans="2:11">
       <c r="B89" s="8">
@@ -3310,15 +3456,16 @@
       <c r="C89" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D89" s="2"/>
+      <c r="E89" s="22"/>
+      <c r="F89" s="22"/>
+      <c r="G89" s="22"/>
+      <c r="H89" s="22"/>
+      <c r="I89" s="22"/>
+      <c r="J89" s="22"/>
+      <c r="K89" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
     </row>
     <row r="90" spans="2:11">
       <c r="B90" s="8">
@@ -3327,15 +3474,16 @@
       <c r="C90" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D90" s="2"/>
+      <c r="E90" s="22"/>
+      <c r="F90" s="22"/>
+      <c r="G90" s="22"/>
+      <c r="H90" s="22"/>
+      <c r="I90" s="22"/>
+      <c r="J90" s="22"/>
+      <c r="K90" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-      <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
     </row>
     <row r="91" spans="2:11">
       <c r="B91" s="8">
@@ -3344,15 +3492,16 @@
       <c r="C91" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D91" s="2"/>
+      <c r="E91" s="22"/>
+      <c r="F91" s="22"/>
+      <c r="G91" s="22"/>
+      <c r="H91" s="22"/>
+      <c r="I91" s="22"/>
+      <c r="J91" s="22"/>
+      <c r="K91" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
     </row>
     <row r="92" spans="2:11">
       <c r="B92" s="8">
@@ -3361,15 +3510,16 @@
       <c r="C92" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D92" s="2"/>
+      <c r="E92" s="22"/>
+      <c r="F92" s="22"/>
+      <c r="G92" s="22"/>
+      <c r="H92" s="22"/>
+      <c r="I92" s="22"/>
+      <c r="J92" s="22"/>
+      <c r="K92" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2"/>
-      <c r="J92" s="2"/>
     </row>
     <row r="93" spans="2:11">
       <c r="B93" s="8">
@@ -3378,15 +3528,16 @@
       <c r="C93" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D93" s="2"/>
+      <c r="E93" s="22"/>
+      <c r="F93" s="22"/>
+      <c r="G93" s="22"/>
+      <c r="H93" s="22"/>
+      <c r="I93" s="22"/>
+      <c r="J93" s="22"/>
+      <c r="K93" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
     </row>
     <row r="94" spans="2:11">
       <c r="B94" s="8">
@@ -3395,15 +3546,16 @@
       <c r="C94" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="D94" s="2"/>
+      <c r="E94" s="22"/>
+      <c r="F94" s="22"/>
+      <c r="G94" s="22"/>
+      <c r="H94" s="22"/>
+      <c r="I94" s="22"/>
+      <c r="J94" s="22"/>
+      <c r="K94" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
-      <c r="J94" s="2"/>
     </row>
     <row r="95" spans="2:11">
       <c r="B95" s="8">
@@ -3412,15 +3564,16 @@
       <c r="C95" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D95" s="2"/>
+      <c r="E95" s="22"/>
+      <c r="F95" s="22"/>
+      <c r="G95" s="22"/>
+      <c r="H95" s="22"/>
+      <c r="I95" s="22"/>
+      <c r="J95" s="22"/>
+      <c r="K95" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-      <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
-      <c r="I95" s="2"/>
-      <c r="J95" s="2"/>
     </row>
     <row r="96" spans="2:11">
       <c r="B96" s="8">
@@ -3429,287 +3582,304 @@
       <c r="C96" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D96" s="2"/>
+      <c r="E96" s="22"/>
+      <c r="F96" s="22"/>
+      <c r="G96" s="22"/>
+      <c r="H96" s="22"/>
+      <c r="I96" s="22"/>
+      <c r="J96" s="22"/>
+      <c r="K96" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="E96" s="2"/>
-      <c r="F96" s="2"/>
-      <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
-      <c r="J96" s="2"/>
-    </row>
-    <row r="97" spans="2:10">
+    </row>
+    <row r="97" spans="2:11">
       <c r="B97" s="8">
         <v>403</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="D97" s="2"/>
+      <c r="E97" s="22"/>
+      <c r="F97" s="22"/>
+      <c r="G97" s="22"/>
+      <c r="H97" s="22"/>
+      <c r="I97" s="22"/>
+      <c r="J97" s="22"/>
+      <c r="K97" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-      <c r="J97" s="2"/>
-    </row>
-    <row r="98" spans="2:10">
+    </row>
+    <row r="98" spans="2:11">
       <c r="B98" s="8">
         <v>410</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D98" s="2"/>
+      <c r="E98" s="22"/>
+      <c r="F98" s="22"/>
+      <c r="G98" s="22"/>
+      <c r="H98" s="22"/>
+      <c r="I98" s="22"/>
+      <c r="J98" s="22"/>
+      <c r="K98" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-      <c r="J98" s="2"/>
-    </row>
-    <row r="99" spans="2:10">
+    </row>
+    <row r="99" spans="2:11">
       <c r="B99" s="8">
         <v>552</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D99" s="2"/>
+      <c r="E99" s="22"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="22"/>
+      <c r="H99" s="22"/>
+      <c r="I99" s="22"/>
+      <c r="J99" s="22"/>
+      <c r="K99" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
-      <c r="I99" s="2"/>
-      <c r="J99" s="2"/>
-    </row>
-    <row r="100" spans="2:10">
+    </row>
+    <row r="100" spans="2:11">
       <c r="B100" s="8">
         <v>312</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D100" s="2"/>
+      <c r="E100" s="22"/>
+      <c r="F100" s="22"/>
+      <c r="G100" s="22"/>
+      <c r="H100" s="22"/>
+      <c r="I100" s="22"/>
+      <c r="J100" s="22"/>
+      <c r="K100" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
-      <c r="J100" s="2"/>
-    </row>
-    <row r="101" spans="2:10">
+    </row>
+    <row r="101" spans="2:11">
       <c r="B101" s="8">
         <v>76</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D101" s="3" t="s">
+      <c r="D101" s="2"/>
+      <c r="E101" s="22"/>
+      <c r="F101" s="22"/>
+      <c r="G101" s="22"/>
+      <c r="H101" s="22"/>
+      <c r="I101" s="22"/>
+      <c r="J101" s="22"/>
+      <c r="K101" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
-      <c r="J101" s="2"/>
-    </row>
-    <row r="102" spans="2:10">
+    </row>
+    <row r="102" spans="2:11">
       <c r="B102" s="8">
         <v>208</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="D102" s="2"/>
+      <c r="E102" s="22"/>
+      <c r="F102" s="22"/>
+      <c r="G102" s="22"/>
+      <c r="H102" s="22"/>
+      <c r="I102" s="22"/>
+      <c r="J102" s="22"/>
+      <c r="K102" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="E102" s="2"/>
-      <c r="F102" s="2"/>
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
-    </row>
-    <row r="103" spans="2:10">
+    </row>
+    <row r="103" spans="2:11">
       <c r="B103" s="8">
         <v>212</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="D103" s="2"/>
+      <c r="E103" s="22"/>
+      <c r="F103" s="22"/>
+      <c r="G103" s="22"/>
+      <c r="H103" s="22"/>
+      <c r="I103" s="22"/>
+      <c r="J103" s="22"/>
+      <c r="K103" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
-      <c r="I103" s="2"/>
-      <c r="J103" s="2"/>
-    </row>
-    <row r="104" spans="2:10">
+    </row>
+    <row r="104" spans="2:11">
       <c r="B104" s="8">
         <v>547</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D104" s="2"/>
+      <c r="E104" s="22"/>
+      <c r="F104" s="22"/>
+      <c r="G104" s="22"/>
+      <c r="H104" s="22"/>
+      <c r="I104" s="22"/>
+      <c r="J104" s="22"/>
+      <c r="K104" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
-    </row>
-    <row r="105" spans="2:10">
+    </row>
+    <row r="105" spans="2:11">
       <c r="B105" s="8">
         <v>130</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D105" s="3" t="s">
+      <c r="D105" s="2"/>
+      <c r="E105" s="22"/>
+      <c r="F105" s="22"/>
+      <c r="G105" s="22"/>
+      <c r="H105" s="22"/>
+      <c r="I105" s="22"/>
+      <c r="J105" s="22"/>
+      <c r="K105" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
-      <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
-      <c r="I105" s="2"/>
-      <c r="J105" s="2"/>
-    </row>
-    <row r="106" spans="2:10">
+    </row>
+    <row r="106" spans="2:11">
       <c r="B106" s="8">
         <v>36</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="D106" s="2"/>
+      <c r="E106" s="22"/>
+      <c r="F106" s="22"/>
+      <c r="G106" s="22"/>
+      <c r="H106" s="22"/>
+      <c r="I106" s="22"/>
+      <c r="J106" s="22"/>
+      <c r="K106" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
-      <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
-      <c r="J106" s="2"/>
-    </row>
-    <row r="107" spans="2:10">
+    </row>
+    <row r="107" spans="2:11">
       <c r="B107" s="8">
         <v>37</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="D107" s="2"/>
+      <c r="E107" s="22"/>
+      <c r="F107" s="22"/>
+      <c r="G107" s="22"/>
+      <c r="H107" s="22"/>
+      <c r="I107" s="22"/>
+      <c r="J107" s="22"/>
+      <c r="K107" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-      <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
-    </row>
-    <row r="108" spans="2:10">
+    </row>
+    <row r="108" spans="2:11">
       <c r="B108" s="8">
         <v>773</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D108" s="3" t="s">
+      <c r="D108" s="2"/>
+      <c r="E108" s="22"/>
+      <c r="F108" s="22"/>
+      <c r="G108" s="22"/>
+      <c r="H108" s="22"/>
+      <c r="I108" s="22"/>
+      <c r="J108" s="22"/>
+      <c r="K108" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-      <c r="J108" s="2"/>
-    </row>
-    <row r="109" spans="2:10">
+    </row>
+    <row r="109" spans="2:11">
       <c r="B109" s="8">
         <v>1091</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="D109" s="2"/>
+      <c r="E109" s="22"/>
+      <c r="F109" s="22"/>
+      <c r="G109" s="22"/>
+      <c r="H109" s="22"/>
+      <c r="I109" s="22"/>
+      <c r="J109" s="22"/>
+      <c r="K109" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-      <c r="G109" s="2"/>
-      <c r="H109" s="2"/>
-      <c r="I109" s="2"/>
-      <c r="J109" s="2"/>
-    </row>
-    <row r="110" spans="2:10">
+    </row>
+    <row r="110" spans="2:11">
       <c r="B110" s="8">
         <v>191</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D110" s="3" t="s">
+      <c r="D110" s="2"/>
+      <c r="E110" s="22"/>
+      <c r="F110" s="22"/>
+      <c r="G110" s="22"/>
+      <c r="H110" s="22"/>
+      <c r="I110" s="22"/>
+      <c r="J110" s="22"/>
+      <c r="K110" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="E110" s="2"/>
-      <c r="F110" s="2"/>
-      <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
-      <c r="J110" s="2"/>
-    </row>
-    <row r="111" spans="2:10">
+    </row>
+    <row r="111" spans="2:11">
       <c r="B111" s="8">
         <v>231</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D111" s="3" t="s">
+      <c r="D111" s="2"/>
+      <c r="E111" s="22"/>
+      <c r="F111" s="22"/>
+      <c r="G111" s="22"/>
+      <c r="H111" s="22"/>
+      <c r="I111" s="22"/>
+      <c r="J111" s="22"/>
+      <c r="K111" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="E111" s="2"/>
-      <c r="F111" s="2"/>
-      <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
-      <c r="I111" s="2"/>
-      <c r="J111" s="2"/>
-    </row>
-    <row r="112" spans="2:10">
+    </row>
+    <row r="112" spans="2:11">
       <c r="B112" s="8">
         <v>190</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D112" s="3" t="s">
+      <c r="D112" s="2"/>
+      <c r="E112" s="22"/>
+      <c r="F112" s="22"/>
+      <c r="G112" s="22"/>
+      <c r="H112" s="22"/>
+      <c r="I112" s="22"/>
+      <c r="J112" s="22"/>
+      <c r="K112" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="E112" s="2"/>
-      <c r="F112" s="2"/>
-      <c r="G112" s="2"/>
-      <c r="H112" s="2"/>
-      <c r="I112" s="2"/>
-      <c r="J112" s="2"/>
     </row>
     <row r="113" spans="2:11">
       <c r="B113" s="8">
@@ -3718,15 +3888,16 @@
       <c r="C113" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D113" s="3" t="s">
+      <c r="D113" s="2"/>
+      <c r="E113" s="22"/>
+      <c r="F113" s="22"/>
+      <c r="G113" s="22"/>
+      <c r="H113" s="22"/>
+      <c r="I113" s="22"/>
+      <c r="J113" s="22"/>
+      <c r="K113" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="E113" s="2"/>
-      <c r="F113" s="2"/>
-      <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
-      <c r="I113" s="2"/>
-      <c r="J113" s="2"/>
     </row>
     <row r="114" spans="2:11">
       <c r="B114" s="8">
@@ -3735,15 +3906,16 @@
       <c r="C114" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D114" s="3" t="s">
+      <c r="D114" s="2"/>
+      <c r="E114" s="22"/>
+      <c r="F114" s="22"/>
+      <c r="G114" s="22"/>
+      <c r="H114" s="22"/>
+      <c r="I114" s="22"/>
+      <c r="J114" s="22"/>
+      <c r="K114" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="E114" s="2"/>
-      <c r="F114" s="2"/>
-      <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
-      <c r="I114" s="2"/>
-      <c r="J114" s="2"/>
     </row>
     <row r="115" spans="2:11">
       <c r="B115" s="8">
@@ -3752,15 +3924,16 @@
       <c r="C115" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D115" s="2"/>
+      <c r="E115" s="22"/>
+      <c r="F115" s="22"/>
+      <c r="G115" s="22"/>
+      <c r="H115" s="22"/>
+      <c r="I115" s="22"/>
+      <c r="J115" s="22"/>
+      <c r="K115" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="E115" s="2"/>
-      <c r="F115" s="2"/>
-      <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
-      <c r="I115" s="2"/>
-      <c r="J115" s="2"/>
     </row>
     <row r="116" spans="2:11">
       <c r="B116" s="8">
@@ -3769,15 +3942,16 @@
       <c r="C116" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="D116" s="2"/>
+      <c r="E116" s="22"/>
+      <c r="F116" s="22"/>
+      <c r="G116" s="22"/>
+      <c r="H116" s="22"/>
+      <c r="I116" s="22"/>
+      <c r="J116" s="22"/>
+      <c r="K116" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2"/>
-      <c r="J116" s="2"/>
     </row>
     <row r="117" spans="2:11">
       <c r="B117" s="8">
@@ -3786,15 +3960,16 @@
       <c r="C117" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D117" s="2"/>
+      <c r="E117" s="22"/>
+      <c r="F117" s="22"/>
+      <c r="G117" s="22"/>
+      <c r="H117" s="22"/>
+      <c r="I117" s="22"/>
+      <c r="J117" s="22"/>
+      <c r="K117" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
-      <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
-      <c r="I117" s="2"/>
-      <c r="J117" s="2"/>
     </row>
     <row r="118" spans="2:11">
       <c r="B118" s="8">
@@ -3803,15 +3978,16 @@
       <c r="C118" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D118" s="2"/>
+      <c r="E118" s="22"/>
+      <c r="F118" s="22"/>
+      <c r="G118" s="22"/>
+      <c r="H118" s="22"/>
+      <c r="I118" s="22"/>
+      <c r="J118" s="22"/>
+      <c r="K118" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="E118" s="2"/>
-      <c r="F118" s="2"/>
-      <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
-      <c r="I118" s="2"/>
-      <c r="J118" s="2"/>
     </row>
     <row r="119" spans="2:11">
       <c r="B119" s="8">
@@ -3820,15 +3996,16 @@
       <c r="C119" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D119" s="3" t="s">
+      <c r="D119" s="2"/>
+      <c r="E119" s="22"/>
+      <c r="F119" s="22"/>
+      <c r="G119" s="22"/>
+      <c r="H119" s="22"/>
+      <c r="I119" s="22"/>
+      <c r="J119" s="22"/>
+      <c r="K119" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="E119" s="2"/>
-      <c r="F119" s="2"/>
-      <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
-      <c r="I119" s="2"/>
-      <c r="J119" s="2"/>
     </row>
     <row r="120" spans="2:11">
       <c r="B120" s="8">
@@ -3837,15 +4014,16 @@
       <c r="C120" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D120" s="3" t="s">
+      <c r="D120" s="2"/>
+      <c r="E120" s="22"/>
+      <c r="F120" s="22"/>
+      <c r="G120" s="22"/>
+      <c r="H120" s="22"/>
+      <c r="I120" s="22"/>
+      <c r="J120" s="22"/>
+      <c r="K120" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E120" s="2"/>
-      <c r="F120" s="2"/>
-      <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
-      <c r="I120" s="2"/>
-      <c r="J120" s="2"/>
     </row>
     <row r="121" spans="2:11">
       <c r="B121" s="8">
@@ -3854,15 +4032,16 @@
       <c r="C121" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D121" s="3" t="s">
+      <c r="D121" s="2"/>
+      <c r="E121" s="22"/>
+      <c r="F121" s="22"/>
+      <c r="G121" s="22"/>
+      <c r="H121" s="22"/>
+      <c r="I121" s="22"/>
+      <c r="J121" s="22"/>
+      <c r="K121" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E121" s="2"/>
-      <c r="F121" s="2"/>
-      <c r="G121" s="2"/>
-      <c r="H121" s="2"/>
-      <c r="I121" s="2"/>
-      <c r="J121" s="2"/>
     </row>
     <row r="122" spans="2:11">
       <c r="B122" s="8">
@@ -3871,15 +4050,16 @@
       <c r="C122" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D122" s="3" t="s">
+      <c r="D122" s="2"/>
+      <c r="E122" s="22"/>
+      <c r="F122" s="22"/>
+      <c r="G122" s="22"/>
+      <c r="H122" s="22"/>
+      <c r="I122" s="22"/>
+      <c r="J122" s="22"/>
+      <c r="K122" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="E122" s="2"/>
-      <c r="F122" s="2"/>
-      <c r="G122" s="2"/>
-      <c r="H122" s="2"/>
-      <c r="I122" s="2"/>
-      <c r="J122" s="2"/>
     </row>
     <row r="123" spans="2:11">
       <c r="B123" s="8">
@@ -3888,16 +4068,16 @@
       <c r="C123" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="D123" s="3" t="s">
+      <c r="D123" s="2"/>
+      <c r="E123" s="22"/>
+      <c r="F123" s="22"/>
+      <c r="G123" s="22"/>
+      <c r="H123" s="22"/>
+      <c r="I123" s="22"/>
+      <c r="J123" s="22"/>
+      <c r="K123" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="E123" s="2"/>
-      <c r="F123" s="2"/>
-      <c r="G123" s="2"/>
-      <c r="H123" s="2"/>
-      <c r="I123" s="2"/>
-      <c r="J123" s="2"/>
-      <c r="K123" s="5"/>
     </row>
     <row r="124" spans="2:11">
       <c r="B124" s="8">
@@ -3906,15 +4086,16 @@
       <c r="C124" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D124" s="3" t="s">
+      <c r="D124" s="2"/>
+      <c r="E124" s="22"/>
+      <c r="F124" s="22"/>
+      <c r="G124" s="22"/>
+      <c r="H124" s="22"/>
+      <c r="I124" s="22"/>
+      <c r="J124" s="22"/>
+      <c r="K124" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="E124" s="2"/>
-      <c r="F124" s="2"/>
-      <c r="G124" s="2"/>
-      <c r="H124" s="2"/>
-      <c r="I124" s="2"/>
-      <c r="J124" s="2"/>
     </row>
     <row r="125" spans="2:11">
       <c r="B125" s="8">
@@ -3923,15 +4104,16 @@
       <c r="C125" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="D125" s="3" t="s">
+      <c r="D125" s="2"/>
+      <c r="E125" s="22"/>
+      <c r="F125" s="22"/>
+      <c r="G125" s="22"/>
+      <c r="H125" s="22"/>
+      <c r="I125" s="22"/>
+      <c r="J125" s="22"/>
+      <c r="K125" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="E125" s="2"/>
-      <c r="F125" s="2"/>
-      <c r="G125" s="2"/>
-      <c r="H125" s="2"/>
-      <c r="I125" s="2"/>
-      <c r="J125" s="2"/>
     </row>
     <row r="126" spans="2:11">
       <c r="B126" s="8">
@@ -3940,15 +4122,16 @@
       <c r="C126" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D126" s="3" t="s">
+      <c r="D126" s="2"/>
+      <c r="E126" s="22"/>
+      <c r="F126" s="22"/>
+      <c r="G126" s="22"/>
+      <c r="H126" s="22"/>
+      <c r="I126" s="22"/>
+      <c r="J126" s="22"/>
+      <c r="K126" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="E126" s="2"/>
-      <c r="F126" s="2"/>
-      <c r="G126" s="2"/>
-      <c r="H126" s="2"/>
-      <c r="I126" s="2"/>
-      <c r="J126" s="2"/>
     </row>
     <row r="127" spans="2:11">
       <c r="B127" s="8">
@@ -3957,15 +4140,16 @@
       <c r="C127" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D127" s="3" t="s">
+      <c r="D127" s="2"/>
+      <c r="E127" s="22"/>
+      <c r="F127" s="22"/>
+      <c r="G127" s="22"/>
+      <c r="H127" s="22"/>
+      <c r="I127" s="22"/>
+      <c r="J127" s="22"/>
+      <c r="K127" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="E127" s="2"/>
-      <c r="F127" s="2"/>
-      <c r="G127" s="2"/>
-      <c r="H127" s="2"/>
-      <c r="I127" s="2"/>
-      <c r="J127" s="2"/>
     </row>
     <row r="128" spans="2:11">
       <c r="B128" s="8">
@@ -3974,363 +4158,376 @@
       <c r="C128" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D128" s="3" t="s">
+      <c r="D128" s="2"/>
+      <c r="E128" s="22"/>
+      <c r="F128" s="22"/>
+      <c r="G128" s="22"/>
+      <c r="H128" s="22"/>
+      <c r="I128" s="22"/>
+      <c r="J128" s="22"/>
+      <c r="K128" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="E128" s="2"/>
-      <c r="F128" s="2"/>
-      <c r="G128" s="2"/>
-      <c r="H128" s="2"/>
-      <c r="I128" s="2"/>
-      <c r="J128" s="2"/>
-    </row>
-    <row r="129" spans="2:10">
+    </row>
+    <row r="129" spans="2:11">
       <c r="B129" s="8">
         <v>771</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D129" s="3" t="s">
+      <c r="D129" s="2"/>
+      <c r="E129" s="22"/>
+      <c r="F129" s="22"/>
+      <c r="G129" s="22"/>
+      <c r="H129" s="22"/>
+      <c r="I129" s="22"/>
+      <c r="J129" s="22"/>
+      <c r="K129" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E129" s="2"/>
-      <c r="F129" s="2"/>
-      <c r="G129" s="2"/>
-      <c r="H129" s="2"/>
-      <c r="I129" s="2"/>
-      <c r="J129" s="2"/>
-    </row>
-    <row r="130" spans="2:10">
+    </row>
+    <row r="130" spans="2:11">
       <c r="B130" s="8">
         <v>387</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D130" s="3" t="s">
+      <c r="D130" s="2"/>
+      <c r="E130" s="22"/>
+      <c r="F130" s="22"/>
+      <c r="G130" s="22"/>
+      <c r="H130" s="22"/>
+      <c r="I130" s="22"/>
+      <c r="J130" s="22"/>
+      <c r="K130" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E130" s="2"/>
-      <c r="F130" s="2"/>
-      <c r="G130" s="2"/>
-      <c r="H130" s="2"/>
-      <c r="I130" s="2"/>
-      <c r="J130" s="2"/>
-    </row>
-    <row r="131" spans="2:10">
+    </row>
+    <row r="131" spans="2:11">
       <c r="B131" s="8">
         <v>14</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="D131" s="3" t="s">
+      <c r="D131" s="2"/>
+      <c r="E131" s="22"/>
+      <c r="F131" s="22"/>
+      <c r="G131" s="22"/>
+      <c r="H131" s="22"/>
+      <c r="I131" s="22"/>
+      <c r="J131" s="22"/>
+      <c r="K131" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="E131" s="2"/>
-      <c r="F131" s="2"/>
-      <c r="G131" s="2"/>
-      <c r="H131" s="2"/>
-      <c r="I131" s="2"/>
-      <c r="J131" s="2"/>
-    </row>
-    <row r="132" spans="2:10">
+    </row>
+    <row r="132" spans="2:11">
       <c r="B132" s="8">
         <v>344</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D132" s="3" t="s">
+      <c r="D132" s="2"/>
+      <c r="E132" s="22"/>
+      <c r="F132" s="22"/>
+      <c r="G132" s="22"/>
+      <c r="H132" s="22"/>
+      <c r="I132" s="22"/>
+      <c r="J132" s="22"/>
+      <c r="K132" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="E132" s="2"/>
-      <c r="F132" s="2"/>
-      <c r="G132" s="2"/>
-      <c r="H132" s="2"/>
-      <c r="I132" s="2"/>
-      <c r="J132" s="2"/>
-    </row>
-    <row r="133" spans="2:10">
+    </row>
+    <row r="133" spans="2:11">
       <c r="B133" s="8">
         <v>541</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D133" s="3" t="s">
+      <c r="D133" s="2"/>
+      <c r="E133" s="22"/>
+      <c r="F133" s="22"/>
+      <c r="G133" s="22"/>
+      <c r="H133" s="22"/>
+      <c r="I133" s="22"/>
+      <c r="J133" s="22"/>
+      <c r="K133" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="E133" s="2"/>
-      <c r="F133" s="2"/>
-      <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
-      <c r="I133" s="2"/>
-      <c r="J133" s="2"/>
-    </row>
-    <row r="134" spans="2:10">
+    </row>
+    <row r="134" spans="2:11">
       <c r="B134" s="8">
         <v>151</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D134" s="3" t="s">
+      <c r="D134" s="2"/>
+      <c r="E134" s="22"/>
+      <c r="F134" s="22"/>
+      <c r="G134" s="22"/>
+      <c r="H134" s="22"/>
+      <c r="I134" s="22"/>
+      <c r="J134" s="22"/>
+      <c r="K134" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="E134" s="2"/>
-      <c r="F134" s="2"/>
-      <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
-      <c r="I134" s="2"/>
-      <c r="J134" s="2"/>
-    </row>
-    <row r="135" spans="2:10">
+    </row>
+    <row r="135" spans="2:11">
       <c r="B135" s="8">
         <v>557</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="D135" s="3" t="s">
+      <c r="D135" s="2"/>
+      <c r="E135" s="22"/>
+      <c r="F135" s="22"/>
+      <c r="G135" s="22"/>
+      <c r="H135" s="22"/>
+      <c r="I135" s="22"/>
+      <c r="J135" s="22"/>
+      <c r="K135" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="E135" s="2"/>
-      <c r="F135" s="2"/>
-      <c r="G135" s="2"/>
-      <c r="H135" s="2"/>
-      <c r="I135" s="2"/>
-      <c r="J135" s="2"/>
-    </row>
-    <row r="136" spans="2:10">
+    </row>
+    <row r="136" spans="2:11">
       <c r="B136" s="8">
         <v>917</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="D136" s="3" t="s">
+      <c r="D136" s="2"/>
+      <c r="E136" s="22"/>
+      <c r="F136" s="22"/>
+      <c r="G136" s="22"/>
+      <c r="H136" s="22"/>
+      <c r="I136" s="22"/>
+      <c r="J136" s="22"/>
+      <c r="K136" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E136" s="2"/>
-      <c r="F136" s="2"/>
-      <c r="G136" s="2"/>
-      <c r="H136" s="2"/>
-      <c r="I136" s="2"/>
-      <c r="J136" s="2"/>
-    </row>
-    <row r="137" spans="2:10">
+    </row>
+    <row r="137" spans="2:11">
       <c r="B137" s="8">
         <v>125</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="D137" s="3" t="s">
+      <c r="D137" s="2"/>
+      <c r="E137" s="22"/>
+      <c r="F137" s="22"/>
+      <c r="G137" s="22"/>
+      <c r="H137" s="22"/>
+      <c r="I137" s="22"/>
+      <c r="J137" s="22"/>
+      <c r="K137" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="E137" s="2"/>
-      <c r="F137" s="2"/>
-      <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
-      <c r="I137" s="2"/>
-      <c r="J137" s="2"/>
-    </row>
-    <row r="138" spans="2:10">
+    </row>
+    <row r="138" spans="2:11">
       <c r="B138" s="8">
         <v>680</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D138" s="3" t="s">
+      <c r="D138" s="2"/>
+      <c r="E138" s="22"/>
+      <c r="F138" s="22"/>
+      <c r="G138" s="22"/>
+      <c r="H138" s="22"/>
+      <c r="I138" s="22"/>
+      <c r="J138" s="22"/>
+      <c r="K138" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="E138" s="2"/>
-      <c r="F138" s="2"/>
-      <c r="G138" s="2"/>
-      <c r="H138" s="2"/>
-      <c r="I138" s="2"/>
-      <c r="J138" s="2"/>
-    </row>
-    <row r="139" spans="2:10">
+    </row>
+    <row r="139" spans="2:11">
       <c r="B139" s="8">
         <v>205</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="D139" s="3" t="s">
+      <c r="D139" s="2"/>
+      <c r="E139" s="22"/>
+      <c r="F139" s="22"/>
+      <c r="G139" s="22"/>
+      <c r="H139" s="22"/>
+      <c r="I139" s="22"/>
+      <c r="J139" s="22"/>
+      <c r="K139" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="E139" s="2"/>
-      <c r="F139" s="2"/>
-      <c r="G139" s="2"/>
-      <c r="H139" s="2"/>
-      <c r="I139" s="2"/>
-      <c r="J139" s="2"/>
-    </row>
-    <row r="140" spans="2:10">
+    </row>
+    <row r="140" spans="2:11">
       <c r="B140" s="8"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
-      <c r="F140" s="2"/>
-      <c r="G140" s="2"/>
-      <c r="H140" s="2"/>
-      <c r="I140" s="2"/>
-      <c r="J140" s="2"/>
-    </row>
-    <row r="141" spans="2:10">
-      <c r="C141" s="14" t="s">
+      <c r="E140" s="22"/>
+      <c r="F140" s="22"/>
+      <c r="G140" s="22"/>
+      <c r="H140" s="22"/>
+      <c r="I140" s="22"/>
+      <c r="J140" s="22"/>
+      <c r="K140" s="2"/>
+    </row>
+    <row r="141" spans="2:11">
+      <c r="C141" s="13" t="s">
         <v>324</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="E1:I1"/>
     <mergeCell ref="A2:A24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="D12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="D13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="D14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="D16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="D17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="D18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="D19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="D20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="D21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="D22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="D23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="D24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="D25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="D26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="D27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="D28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="D29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="D30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="D31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="D32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="D33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="D34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="D35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="D36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="D37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="D38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="D39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="D40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="D41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="D42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="D43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="D44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="D45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="D46" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="D47" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="D48" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="D49" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="D50" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="D51" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="D52" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="D53" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="D54" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="D55" r:id="rId54" location="/description" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="D56" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="D57" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="D58" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
-    <hyperlink ref="D59" r:id="rId58" location="/description" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
-    <hyperlink ref="D60" r:id="rId59" location="/description" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
-    <hyperlink ref="D61" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
-    <hyperlink ref="D62" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
-    <hyperlink ref="D63" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
-    <hyperlink ref="D64" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
-    <hyperlink ref="D65" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
-    <hyperlink ref="D66" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
-    <hyperlink ref="D67" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
-    <hyperlink ref="D68" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
-    <hyperlink ref="D69" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
-    <hyperlink ref="D71" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
-    <hyperlink ref="D72" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
-    <hyperlink ref="D73" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
-    <hyperlink ref="D74" r:id="rId72" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
-    <hyperlink ref="D75" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
-    <hyperlink ref="D76" r:id="rId74" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
-    <hyperlink ref="D77" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
-    <hyperlink ref="D78" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
-    <hyperlink ref="D80" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
-    <hyperlink ref="D81" r:id="rId78" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
-    <hyperlink ref="D82" r:id="rId79" location="/description" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
-    <hyperlink ref="D83" r:id="rId80" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
-    <hyperlink ref="D84" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
-    <hyperlink ref="D85" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
-    <hyperlink ref="D86" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
-    <hyperlink ref="D87" r:id="rId84" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
-    <hyperlink ref="D88" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
-    <hyperlink ref="D89" r:id="rId86" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
-    <hyperlink ref="D79" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
-    <hyperlink ref="D90" r:id="rId88" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
-    <hyperlink ref="D91" r:id="rId89" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
-    <hyperlink ref="D92" r:id="rId90" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
-    <hyperlink ref="D93" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
-    <hyperlink ref="D94" r:id="rId92" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
-    <hyperlink ref="D95" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
-    <hyperlink ref="D96" r:id="rId94" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
-    <hyperlink ref="D97" r:id="rId95" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
-    <hyperlink ref="D98" r:id="rId96" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
-    <hyperlink ref="D99" r:id="rId97" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
-    <hyperlink ref="D100" r:id="rId98" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
-    <hyperlink ref="D101" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
-    <hyperlink ref="D102" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
-    <hyperlink ref="D103" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
-    <hyperlink ref="D104" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
-    <hyperlink ref="D105" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
-    <hyperlink ref="D106" r:id="rId104" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
-    <hyperlink ref="D107" r:id="rId105" location="/description" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
-    <hyperlink ref="D108" r:id="rId106" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
-    <hyperlink ref="D109" r:id="rId107" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
-    <hyperlink ref="D110" r:id="rId108" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
-    <hyperlink ref="D111" r:id="rId109" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
-    <hyperlink ref="D112" r:id="rId110" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
-    <hyperlink ref="D113" r:id="rId111" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
-    <hyperlink ref="D114" r:id="rId112" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
-    <hyperlink ref="D115" r:id="rId113" location="/" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
-    <hyperlink ref="D116" r:id="rId114" xr:uid="{00000000-0004-0000-0100-000071000000}"/>
-    <hyperlink ref="D117" r:id="rId115" xr:uid="{00000000-0004-0000-0100-000072000000}"/>
-    <hyperlink ref="D118" r:id="rId116" xr:uid="{00000000-0004-0000-0100-000073000000}"/>
-    <hyperlink ref="D119" r:id="rId117" xr:uid="{00000000-0004-0000-0100-000074000000}"/>
-    <hyperlink ref="D120" r:id="rId118" xr:uid="{00000000-0004-0000-0100-000075000000}"/>
-    <hyperlink ref="D121" r:id="rId119" xr:uid="{00000000-0004-0000-0100-000076000000}"/>
-    <hyperlink ref="D123" r:id="rId120" xr:uid="{00000000-0004-0000-0100-000077000000}"/>
-    <hyperlink ref="D122" r:id="rId121" xr:uid="{00000000-0004-0000-0100-000078000000}"/>
-    <hyperlink ref="D124" r:id="rId122" xr:uid="{00000000-0004-0000-0100-000079000000}"/>
-    <hyperlink ref="D125" r:id="rId123" xr:uid="{00000000-0004-0000-0100-00007A000000}"/>
-    <hyperlink ref="D126" r:id="rId124" xr:uid="{00000000-0004-0000-0100-00007B000000}"/>
-    <hyperlink ref="D127" r:id="rId125" xr:uid="{00000000-0004-0000-0100-00007C000000}"/>
-    <hyperlink ref="D128" r:id="rId126" xr:uid="{00000000-0004-0000-0100-00007D000000}"/>
-    <hyperlink ref="D129" r:id="rId127" xr:uid="{00000000-0004-0000-0100-00007E000000}"/>
-    <hyperlink ref="D130" r:id="rId128" xr:uid="{00000000-0004-0000-0100-00007F000000}"/>
-    <hyperlink ref="D131" r:id="rId129" xr:uid="{00000000-0004-0000-0100-000080000000}"/>
-    <hyperlink ref="D132" r:id="rId130" xr:uid="{00000000-0004-0000-0100-000081000000}"/>
-    <hyperlink ref="D133" r:id="rId131" xr:uid="{00000000-0004-0000-0100-000082000000}"/>
-    <hyperlink ref="D134" r:id="rId132" xr:uid="{00000000-0004-0000-0100-000083000000}"/>
-    <hyperlink ref="D135" r:id="rId133" xr:uid="{00000000-0004-0000-0100-000084000000}"/>
-    <hyperlink ref="D136" r:id="rId134" xr:uid="{00000000-0004-0000-0100-000085000000}"/>
-    <hyperlink ref="D137" r:id="rId135" xr:uid="{00000000-0004-0000-0100-000086000000}"/>
-    <hyperlink ref="D138" r:id="rId136" xr:uid="{00000000-0004-0000-0100-000087000000}"/>
-    <hyperlink ref="D139" r:id="rId137" xr:uid="{00000000-0004-0000-0100-000088000000}"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="K4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="K5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="K6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="K7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="K8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="K9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="K10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="K11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="K12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="K13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="K14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="K15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="K16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="K17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="K18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="K19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="K20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="K21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="K22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="K23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="K24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="K25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="K26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="K27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="K28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="K29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="K30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="K31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="K32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="K33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="K34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="K35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="K36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="K37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="K38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="K39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="K40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="K41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="K42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="K43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="K44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="K45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="K46" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="K47" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="K48" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="K49" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="K50" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="K51" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="K52" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="K53" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="K54" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="K55" r:id="rId54" location="/description" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="K56" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="K57" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="K58" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="K59" r:id="rId58" location="/description" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="K60" r:id="rId59" location="/description" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="K61" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="K62" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="K63" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="K64" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="K65" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="K66" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="K67" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="K68" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="K69" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="K71" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="K72" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="K73" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="K74" r:id="rId72" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="K75" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="K76" r:id="rId74" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="K77" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="K78" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="K80" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="K81" r:id="rId78" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="K82" r:id="rId79" location="/description" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="K83" r:id="rId80" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="K84" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="K85" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="K86" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="K87" r:id="rId84" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="K88" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="K89" r:id="rId86" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
+    <hyperlink ref="K79" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
+    <hyperlink ref="K90" r:id="rId88" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
+    <hyperlink ref="K91" r:id="rId89" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
+    <hyperlink ref="K92" r:id="rId90" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
+    <hyperlink ref="K93" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
+    <hyperlink ref="K94" r:id="rId92" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
+    <hyperlink ref="K95" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
+    <hyperlink ref="K96" r:id="rId94" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
+    <hyperlink ref="K97" r:id="rId95" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
+    <hyperlink ref="K98" r:id="rId96" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
+    <hyperlink ref="K99" r:id="rId97" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
+    <hyperlink ref="K100" r:id="rId98" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
+    <hyperlink ref="K101" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
+    <hyperlink ref="K102" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
+    <hyperlink ref="K103" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="K104" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="K105" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
+    <hyperlink ref="K106" r:id="rId104" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
+    <hyperlink ref="K107" r:id="rId105" location="/description" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
+    <hyperlink ref="K108" r:id="rId106" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
+    <hyperlink ref="K109" r:id="rId107" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
+    <hyperlink ref="K110" r:id="rId108" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
+    <hyperlink ref="K111" r:id="rId109" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
+    <hyperlink ref="K112" r:id="rId110" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
+    <hyperlink ref="K113" r:id="rId111" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
+    <hyperlink ref="K114" r:id="rId112" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
+    <hyperlink ref="K115" r:id="rId113" location="/" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
+    <hyperlink ref="K116" r:id="rId114" xr:uid="{00000000-0004-0000-0100-000071000000}"/>
+    <hyperlink ref="K117" r:id="rId115" xr:uid="{00000000-0004-0000-0100-000072000000}"/>
+    <hyperlink ref="K118" r:id="rId116" xr:uid="{00000000-0004-0000-0100-000073000000}"/>
+    <hyperlink ref="K119" r:id="rId117" xr:uid="{00000000-0004-0000-0100-000074000000}"/>
+    <hyperlink ref="K120" r:id="rId118" xr:uid="{00000000-0004-0000-0100-000075000000}"/>
+    <hyperlink ref="K121" r:id="rId119" xr:uid="{00000000-0004-0000-0100-000076000000}"/>
+    <hyperlink ref="K123" r:id="rId120" xr:uid="{00000000-0004-0000-0100-000077000000}"/>
+    <hyperlink ref="K122" r:id="rId121" xr:uid="{00000000-0004-0000-0100-000078000000}"/>
+    <hyperlink ref="K124" r:id="rId122" xr:uid="{00000000-0004-0000-0100-000079000000}"/>
+    <hyperlink ref="K125" r:id="rId123" xr:uid="{00000000-0004-0000-0100-00007A000000}"/>
+    <hyperlink ref="K126" r:id="rId124" xr:uid="{00000000-0004-0000-0100-00007B000000}"/>
+    <hyperlink ref="K127" r:id="rId125" xr:uid="{00000000-0004-0000-0100-00007C000000}"/>
+    <hyperlink ref="K128" r:id="rId126" xr:uid="{00000000-0004-0000-0100-00007D000000}"/>
+    <hyperlink ref="K129" r:id="rId127" xr:uid="{00000000-0004-0000-0100-00007E000000}"/>
+    <hyperlink ref="K130" r:id="rId128" xr:uid="{00000000-0004-0000-0100-00007F000000}"/>
+    <hyperlink ref="K131" r:id="rId129" xr:uid="{00000000-0004-0000-0100-000080000000}"/>
+    <hyperlink ref="K132" r:id="rId130" xr:uid="{00000000-0004-0000-0100-000081000000}"/>
+    <hyperlink ref="K133" r:id="rId131" xr:uid="{00000000-0004-0000-0100-000082000000}"/>
+    <hyperlink ref="K134" r:id="rId132" xr:uid="{00000000-0004-0000-0100-000083000000}"/>
+    <hyperlink ref="K135" r:id="rId133" xr:uid="{00000000-0004-0000-0100-000084000000}"/>
+    <hyperlink ref="K136" r:id="rId134" xr:uid="{00000000-0004-0000-0100-000085000000}"/>
+    <hyperlink ref="K137" r:id="rId135" xr:uid="{00000000-0004-0000-0100-000086000000}"/>
+    <hyperlink ref="K138" r:id="rId136" xr:uid="{00000000-0004-0000-0100-000087000000}"/>
+    <hyperlink ref="K139" r:id="rId137" xr:uid="{00000000-0004-0000-0100-000088000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId138"/>
@@ -4368,13 +4565,13 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">

</xml_diff>

<commit_message>
Q25 这道题理解啦 ！！！！ 最关键的 pre,end,stat,next;  ListNode pre = dummy;  ListNode end = dummy;
</commit_message>
<xml_diff>
--- a/code/src/main/leetcode.xlsx
+++ b/code/src/main/leetcode.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A1A6E6-2FDE-B344-A638-83495EC7290E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10F1942-E61B-5F43-A9FD-9FDEBC90BA6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1334,7 +1334,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -1511,6 +1511,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1518,22 +1534,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1818,18 +1818,18 @@
   <dimension ref="A1:K141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="20.1640625" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="24" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="24" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="24" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.83203125" style="24"/>
+    <col min="5" max="5" width="13.1640625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="18" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.83203125" style="18"/>
     <col min="11" max="11" width="106.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1843,20 +1843,20 @@
       <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="25"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="19"/>
       <c r="K1" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="24" t="s">
         <v>329</v>
       </c>
       <c r="B2">
@@ -1866,18 +1866,18 @@
         <v>57</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
       <c r="K2" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="16"/>
+      <c r="A3" s="24"/>
       <c r="B3">
         <v>1</v>
       </c>
@@ -1885,20 +1885,20 @@
         <v>30</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16">
         <v>44074</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
       <c r="K3" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="16"/>
+      <c r="A4" s="24"/>
       <c r="B4">
         <v>283</v>
       </c>
@@ -1906,18 +1906,18 @@
         <v>16</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="16"/>
+      <c r="A5" s="24"/>
       <c r="B5">
         <v>70</v>
       </c>
@@ -1925,18 +1925,18 @@
         <v>54</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
       <c r="K5" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="16"/>
+      <c r="A6" s="24"/>
       <c r="B6">
         <v>15</v>
       </c>
@@ -1944,24 +1944,24 @@
         <v>49</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="22">
+      <c r="E6" s="16">
         <v>44006</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="16">
         <v>44042</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="16">
         <v>44074</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
       <c r="K6" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="16"/>
+      <c r="A7" s="24"/>
       <c r="B7">
         <v>11</v>
       </c>
@@ -1969,26 +1969,26 @@
         <v>60</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="22">
+      <c r="E7" s="16">
         <v>44006</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="16">
         <v>44040</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="16">
         <v>44074</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="16" t="s">
         <v>330</v>
       </c>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
       <c r="K7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="16"/>
+      <c r="A8" s="24"/>
       <c r="B8">
         <v>206</v>
       </c>
@@ -1996,17 +1996,17 @@
         <v>18</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
       <c r="K8" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="16"/>
+      <c r="A9" s="24"/>
       <c r="B9">
         <v>24</v>
       </c>
@@ -2014,20 +2014,20 @@
         <v>8</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="26">
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="20">
         <v>44074</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
       <c r="K9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="16"/>
+      <c r="A10" s="24"/>
       <c r="B10">
         <v>141</v>
       </c>
@@ -2035,18 +2035,18 @@
         <v>46</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
       <c r="K10" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="16"/>
+      <c r="A11" s="24"/>
       <c r="B11">
         <v>142</v>
       </c>
@@ -2054,18 +2054,18 @@
         <v>63</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
       <c r="K11" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="16"/>
+      <c r="A12" s="24"/>
       <c r="B12">
         <v>25</v>
       </c>
@@ -2073,18 +2073,24 @@
         <v>65</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16">
+        <v>44049</v>
+      </c>
+      <c r="G12" s="16">
+        <v>44075</v>
+      </c>
+      <c r="H12" s="16">
+        <v>44076</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
       <c r="K12" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="16"/>
+      <c r="A13" s="24"/>
       <c r="B13">
         <v>20</v>
       </c>
@@ -2092,18 +2098,18 @@
         <v>37</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
       <c r="K13" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="16"/>
+      <c r="A14" s="24"/>
       <c r="B14">
         <v>155</v>
       </c>
@@ -2111,18 +2117,18 @@
         <v>40</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
       <c r="K14" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="16"/>
+      <c r="A15" s="24"/>
       <c r="B15">
         <v>84</v>
       </c>
@@ -2130,18 +2136,18 @@
         <v>47</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
       <c r="K15" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="16"/>
+      <c r="A16" s="24"/>
       <c r="B16">
         <v>239</v>
       </c>
@@ -2149,18 +2155,18 @@
         <v>41</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
       <c r="K16" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="16"/>
+      <c r="A17" s="24"/>
       <c r="B17">
         <v>641</v>
       </c>
@@ -2168,18 +2174,18 @@
         <v>34</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
       <c r="K17" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="16"/>
+      <c r="A18" s="24"/>
       <c r="B18">
         <v>42</v>
       </c>
@@ -2187,18 +2193,18 @@
         <v>36</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
       <c r="K18" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="16"/>
+      <c r="A19" s="24"/>
       <c r="B19">
         <v>26</v>
       </c>
@@ -2206,18 +2212,18 @@
         <v>26</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
       <c r="K19" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="16"/>
+      <c r="A20" s="24"/>
       <c r="B20">
         <v>189</v>
       </c>
@@ -2225,18 +2231,18 @@
         <v>21</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
       <c r="K20" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="16"/>
+      <c r="A21" s="24"/>
       <c r="B21">
         <v>21</v>
       </c>
@@ -2244,22 +2250,22 @@
         <v>25</v>
       </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="22">
+      <c r="E21" s="16">
         <v>44054</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="16">
         <v>44074</v>
       </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
       <c r="K21" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="16"/>
+      <c r="A22" s="24"/>
       <c r="B22">
         <v>88</v>
       </c>
@@ -2267,18 +2273,18 @@
         <v>28</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
       <c r="K22" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="16"/>
+      <c r="A23" s="24"/>
       <c r="B23">
         <v>66</v>
       </c>
@@ -2286,18 +2292,18 @@
         <v>31</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
       <c r="K23" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="17"/>
+      <c r="A24" s="25"/>
       <c r="B24">
         <v>242</v>
       </c>
@@ -2305,12 +2311,12 @@
         <v>72</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
       <c r="K24" s="3" t="s">
         <v>71</v>
       </c>
@@ -2324,12 +2330,12 @@
         <v>321</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
       <c r="K25" s="3" t="s">
         <v>73</v>
       </c>
@@ -2342,12 +2348,12 @@
         <v>75</v>
       </c>
       <c r="D26" s="2"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
       <c r="K26" s="3" t="s">
         <v>74</v>
       </c>
@@ -2360,12 +2366,12 @@
         <v>322</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
       <c r="K27" s="3" t="s">
         <v>76</v>
       </c>
@@ -2378,12 +2384,12 @@
         <v>78</v>
       </c>
       <c r="D28" s="2"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
       <c r="K28" s="3" t="s">
         <v>77</v>
       </c>
@@ -2396,12 +2402,12 @@
         <v>80</v>
       </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
       <c r="K29" s="3" t="s">
         <v>79</v>
       </c>
@@ -2414,12 +2420,12 @@
         <v>82</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
       <c r="K30" s="3" t="s">
         <v>81</v>
       </c>
@@ -2432,12 +2438,12 @@
         <v>83</v>
       </c>
       <c r="D31" s="2"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
       <c r="K31" s="3" t="s">
         <v>323</v>
       </c>
@@ -2450,12 +2456,12 @@
         <v>85</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
       <c r="K32" s="3" t="s">
         <v>84</v>
       </c>
@@ -2468,12 +2474,12 @@
         <v>87</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
       <c r="K33" s="3" t="s">
         <v>86</v>
       </c>
@@ -2486,12 +2492,12 @@
         <v>89</v>
       </c>
       <c r="D34" s="2"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
       <c r="K34" s="3" t="s">
         <v>88</v>
       </c>
@@ -2504,12 +2510,12 @@
         <v>91</v>
       </c>
       <c r="D35" s="2"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
       <c r="K35" s="3" t="s">
         <v>90</v>
       </c>
@@ -2522,12 +2528,12 @@
         <v>93</v>
       </c>
       <c r="D36" s="2"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
       <c r="K36" s="3" t="s">
         <v>328</v>
       </c>
@@ -2540,12 +2546,12 @@
         <v>95</v>
       </c>
       <c r="D37" s="2"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
       <c r="K37" s="3" t="s">
         <v>94</v>
       </c>
@@ -2558,12 +2564,12 @@
         <v>97</v>
       </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
       <c r="K38" s="3" t="s">
         <v>96</v>
       </c>
@@ -2576,12 +2582,12 @@
         <v>99</v>
       </c>
       <c r="D39" s="2"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
       <c r="K39" s="3" t="s">
         <v>98</v>
       </c>
@@ -2594,12 +2600,12 @@
         <v>10</v>
       </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
       <c r="K40" s="3" t="s">
         <v>100</v>
       </c>
@@ -2612,12 +2618,12 @@
         <v>14</v>
       </c>
       <c r="D41" s="2"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
       <c r="K41" s="3" t="s">
         <v>13</v>
       </c>
@@ -2630,12 +2636,12 @@
         <v>102</v>
       </c>
       <c r="D42" s="2"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
       <c r="K42" s="3" t="s">
         <v>101</v>
       </c>
@@ -2648,12 +2654,12 @@
         <v>104</v>
       </c>
       <c r="D43" s="2"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
       <c r="K43" s="3" t="s">
         <v>103</v>
       </c>
@@ -2666,12 +2672,12 @@
         <v>106</v>
       </c>
       <c r="D44" s="2"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
       <c r="K44" s="3" t="s">
         <v>105</v>
       </c>
@@ -2684,12 +2690,12 @@
         <v>108</v>
       </c>
       <c r="D45" s="2"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
       <c r="K45" s="3" t="s">
         <v>107</v>
       </c>
@@ -2702,12 +2708,12 @@
         <v>110</v>
       </c>
       <c r="D46" s="2"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
       <c r="K46" s="3" t="s">
         <v>109</v>
       </c>
@@ -2720,12 +2726,12 @@
         <v>112</v>
       </c>
       <c r="D47" s="2"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
       <c r="K47" s="3" t="s">
         <v>111</v>
       </c>
@@ -2738,12 +2744,12 @@
         <v>114</v>
       </c>
       <c r="D48" s="2"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
       <c r="K48" s="3" t="s">
         <v>113</v>
       </c>
@@ -2756,12 +2762,12 @@
         <v>116</v>
       </c>
       <c r="D49" s="2"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
       <c r="K49" s="3" t="s">
         <v>115</v>
       </c>
@@ -2774,12 +2780,12 @@
         <v>118</v>
       </c>
       <c r="D50" s="2"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
       <c r="K50" s="3" t="s">
         <v>117</v>
       </c>
@@ -2792,12 +2798,12 @@
         <v>120</v>
       </c>
       <c r="D51" s="2"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
       <c r="K51" s="3" t="s">
         <v>119</v>
       </c>
@@ -2810,12 +2816,12 @@
         <v>122</v>
       </c>
       <c r="D52" s="2"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="22"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
       <c r="K52" s="3" t="s">
         <v>121</v>
       </c>
@@ -2828,12 +2834,12 @@
         <v>124</v>
       </c>
       <c r="D53" s="2"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="22"/>
-      <c r="I53" s="22"/>
-      <c r="J53" s="22"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
       <c r="K53" s="3" t="s">
         <v>123</v>
       </c>
@@ -2846,12 +2852,12 @@
         <v>126</v>
       </c>
       <c r="D54" s="2"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="22"/>
-      <c r="J54" s="22"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
       <c r="K54" s="3" t="s">
         <v>125</v>
       </c>
@@ -2864,12 +2870,12 @@
         <v>128</v>
       </c>
       <c r="D55" s="2"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
-      <c r="H55" s="22"/>
-      <c r="I55" s="22"/>
-      <c r="J55" s="22"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
       <c r="K55" s="3" t="s">
         <v>127</v>
       </c>
@@ -2882,12 +2888,12 @@
         <v>130</v>
       </c>
       <c r="D56" s="2"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="22"/>
-      <c r="G56" s="22"/>
-      <c r="H56" s="22"/>
-      <c r="I56" s="22"/>
-      <c r="J56" s="22"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
       <c r="K56" s="3" t="s">
         <v>129</v>
       </c>
@@ -2900,12 +2906,12 @@
         <v>133</v>
       </c>
       <c r="D57" s="2"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
-      <c r="H57" s="22"/>
-      <c r="I57" s="22"/>
-      <c r="J57" s="22"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
       <c r="K57" s="3" t="s">
         <v>131</v>
       </c>
@@ -2918,12 +2924,12 @@
         <v>132</v>
       </c>
       <c r="D58" s="2"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="22"/>
-      <c r="H58" s="22"/>
-      <c r="I58" s="22"/>
-      <c r="J58" s="22"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
       <c r="K58" s="3" t="s">
         <v>134</v>
       </c>
@@ -2936,12 +2942,12 @@
         <v>136</v>
       </c>
       <c r="D59" s="2"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="22"/>
-      <c r="J59" s="22"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
       <c r="K59" s="3" t="s">
         <v>135</v>
       </c>
@@ -2954,12 +2960,12 @@
         <v>138</v>
       </c>
       <c r="D60" s="2"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
-      <c r="I60" s="22"/>
-      <c r="J60" s="22"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
       <c r="K60" s="3" t="s">
         <v>137</v>
       </c>
@@ -2972,12 +2978,12 @@
         <v>140</v>
       </c>
       <c r="D61" s="2"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="22"/>
-      <c r="G61" s="22"/>
-      <c r="H61" s="22"/>
-      <c r="I61" s="22"/>
-      <c r="J61" s="22"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
       <c r="K61" s="3" t="s">
         <v>139</v>
       </c>
@@ -2990,12 +2996,12 @@
         <v>142</v>
       </c>
       <c r="D62" s="2"/>
-      <c r="E62" s="22"/>
-      <c r="F62" s="22"/>
-      <c r="G62" s="22"/>
-      <c r="H62" s="22"/>
-      <c r="I62" s="22"/>
-      <c r="J62" s="22"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
       <c r="K62" s="3" t="s">
         <v>141</v>
       </c>
@@ -3008,12 +3014,12 @@
         <v>144</v>
       </c>
       <c r="D63" s="2"/>
-      <c r="E63" s="22"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="22"/>
-      <c r="I63" s="22"/>
-      <c r="J63" s="22"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="16"/>
       <c r="K63" s="3" t="s">
         <v>143</v>
       </c>
@@ -3026,12 +3032,12 @@
         <v>148</v>
       </c>
       <c r="D64" s="2"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="22"/>
-      <c r="G64" s="22"/>
-      <c r="H64" s="22"/>
-      <c r="I64" s="22"/>
-      <c r="J64" s="22"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+      <c r="I64" s="16"/>
+      <c r="J64" s="16"/>
       <c r="K64" s="3" t="s">
         <v>147</v>
       </c>
@@ -3044,12 +3050,12 @@
         <v>150</v>
       </c>
       <c r="D65" s="2"/>
-      <c r="E65" s="22"/>
-      <c r="F65" s="22"/>
-      <c r="G65" s="22"/>
-      <c r="H65" s="22"/>
-      <c r="I65" s="22"/>
-      <c r="J65" s="22"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
       <c r="K65" s="3" t="s">
         <v>149</v>
       </c>
@@ -3062,12 +3068,12 @@
         <v>152</v>
       </c>
       <c r="D66" s="2"/>
-      <c r="E66" s="22"/>
-      <c r="F66" s="22"/>
-      <c r="G66" s="22"/>
-      <c r="H66" s="22"/>
-      <c r="I66" s="22"/>
-      <c r="J66" s="22"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+      <c r="I66" s="16"/>
+      <c r="J66" s="16"/>
       <c r="K66" s="3" t="s">
         <v>151</v>
       </c>
@@ -3080,12 +3086,12 @@
         <v>153</v>
       </c>
       <c r="D67" s="2"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="22"/>
-      <c r="G67" s="22"/>
-      <c r="H67" s="22"/>
-      <c r="I67" s="22"/>
-      <c r="J67" s="22"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
       <c r="K67" s="3" t="s">
         <v>55</v>
       </c>
@@ -3098,12 +3104,12 @@
         <v>155</v>
       </c>
       <c r="D68" s="2"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="22"/>
-      <c r="G68" s="22"/>
-      <c r="H68" s="22"/>
-      <c r="I68" s="22"/>
-      <c r="J68" s="22"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+      <c r="I68" s="16"/>
+      <c r="J68" s="16"/>
       <c r="K68" s="3" t="s">
         <v>154</v>
       </c>
@@ -3116,12 +3122,12 @@
         <v>157</v>
       </c>
       <c r="D69" s="2"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="22"/>
-      <c r="G69" s="22"/>
-      <c r="H69" s="22"/>
-      <c r="I69" s="22"/>
-      <c r="J69" s="22"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+      <c r="I69" s="16"/>
+      <c r="J69" s="16"/>
       <c r="K69" s="3" t="s">
         <v>156</v>
       </c>
@@ -3129,12 +3135,12 @@
     <row r="70" spans="2:11">
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="22"/>
-      <c r="F70" s="22"/>
-      <c r="G70" s="22"/>
-      <c r="H70" s="22"/>
-      <c r="I70" s="22"/>
-      <c r="J70" s="22"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+      <c r="I70" s="16"/>
+      <c r="J70" s="16"/>
       <c r="K70" s="2"/>
     </row>
     <row r="71" spans="2:11">
@@ -3145,12 +3151,12 @@
         <v>165</v>
       </c>
       <c r="D71" s="2"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="22"/>
-      <c r="G71" s="22"/>
-      <c r="H71" s="22"/>
-      <c r="I71" s="22"/>
-      <c r="J71" s="22"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
       <c r="K71" s="3" t="s">
         <v>166</v>
       </c>
@@ -3163,12 +3169,12 @@
         <v>167</v>
       </c>
       <c r="D72" s="2"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="22"/>
-      <c r="G72" s="22"/>
-      <c r="H72" s="22"/>
-      <c r="I72" s="22"/>
-      <c r="J72" s="22"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="16"/>
+      <c r="I72" s="16"/>
+      <c r="J72" s="16"/>
       <c r="K72" s="3" t="s">
         <v>168</v>
       </c>
@@ -3181,12 +3187,12 @@
         <v>159</v>
       </c>
       <c r="D73" s="2"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="22"/>
-      <c r="G73" s="22"/>
-      <c r="H73" s="22"/>
-      <c r="I73" s="22"/>
-      <c r="J73" s="22"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="16"/>
+      <c r="J73" s="16"/>
       <c r="K73" s="3" t="s">
         <v>158</v>
       </c>
@@ -3199,12 +3205,12 @@
         <v>54</v>
       </c>
       <c r="D74" s="2"/>
-      <c r="E74" s="22"/>
-      <c r="F74" s="22"/>
-      <c r="G74" s="22"/>
-      <c r="H74" s="22"/>
-      <c r="I74" s="22"/>
-      <c r="J74" s="22"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
       <c r="K74" s="3" t="s">
         <v>169</v>
       </c>
@@ -3217,12 +3223,12 @@
         <v>161</v>
       </c>
       <c r="D75" s="2"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="22"/>
-      <c r="G75" s="22"/>
-      <c r="H75" s="22"/>
-      <c r="I75" s="22"/>
-      <c r="J75" s="22"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
+      <c r="J75" s="16"/>
       <c r="K75" s="3" t="s">
         <v>160</v>
       </c>
@@ -3235,12 +3241,12 @@
         <v>170</v>
       </c>
       <c r="D76" s="2"/>
-      <c r="E76" s="22"/>
-      <c r="F76" s="22"/>
-      <c r="G76" s="22"/>
-      <c r="H76" s="22"/>
-      <c r="I76" s="22"/>
-      <c r="J76" s="22"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="16"/>
+      <c r="I76" s="16"/>
+      <c r="J76" s="16"/>
       <c r="K76" s="3" t="s">
         <v>162</v>
       </c>
@@ -3253,12 +3259,12 @@
         <v>171</v>
       </c>
       <c r="D77" s="2"/>
-      <c r="E77" s="22"/>
-      <c r="F77" s="22"/>
-      <c r="G77" s="22"/>
-      <c r="H77" s="22"/>
-      <c r="I77" s="22"/>
-      <c r="J77" s="22"/>
+      <c r="E77" s="16"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="16"/>
+      <c r="I77" s="16"/>
+      <c r="J77" s="16"/>
       <c r="K77" s="3" t="s">
         <v>172</v>
       </c>
@@ -3271,12 +3277,12 @@
         <v>146</v>
       </c>
       <c r="D78" s="2"/>
-      <c r="E78" s="22"/>
-      <c r="F78" s="22"/>
-      <c r="G78" s="22"/>
-      <c r="H78" s="22"/>
-      <c r="I78" s="22"/>
-      <c r="J78" s="22"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="16"/>
+      <c r="I78" s="16"/>
+      <c r="J78" s="16"/>
       <c r="K78" s="3" t="s">
         <v>173</v>
       </c>
@@ -3289,12 +3295,12 @@
         <v>174</v>
       </c>
       <c r="D79" s="2"/>
-      <c r="E79" s="22"/>
-      <c r="F79" s="22"/>
-      <c r="G79" s="22"/>
-      <c r="H79" s="22"/>
-      <c r="I79" s="22"/>
-      <c r="J79" s="22"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="16"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="16"/>
+      <c r="I79" s="16"/>
+      <c r="J79" s="16"/>
       <c r="K79" s="3" t="s">
         <v>175</v>
       </c>
@@ -3307,12 +3313,12 @@
         <v>164</v>
       </c>
       <c r="D80" s="2"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="22"/>
-      <c r="G80" s="22"/>
-      <c r="H80" s="22"/>
-      <c r="I80" s="22"/>
-      <c r="J80" s="22"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="16"/>
+      <c r="I80" s="16"/>
+      <c r="J80" s="16"/>
       <c r="K80" s="3" t="s">
         <v>163</v>
       </c>
@@ -3325,12 +3331,12 @@
         <v>176</v>
       </c>
       <c r="D81" s="2"/>
-      <c r="E81" s="22"/>
-      <c r="F81" s="22"/>
-      <c r="G81" s="22"/>
-      <c r="H81" s="22"/>
-      <c r="I81" s="22"/>
-      <c r="J81" s="22"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
+      <c r="J81" s="16"/>
       <c r="K81" s="3" t="s">
         <v>177</v>
       </c>
@@ -3343,12 +3349,12 @@
         <v>178</v>
       </c>
       <c r="D82" s="2"/>
-      <c r="E82" s="22"/>
-      <c r="F82" s="22"/>
-      <c r="G82" s="22"/>
-      <c r="H82" s="22"/>
-      <c r="I82" s="22"/>
-      <c r="J82" s="22"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="16"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+      <c r="J82" s="16"/>
       <c r="K82" s="3" t="s">
         <v>179</v>
       </c>
@@ -3361,12 +3367,12 @@
         <v>180</v>
       </c>
       <c r="D83" s="2"/>
-      <c r="E83" s="22"/>
-      <c r="F83" s="22"/>
-      <c r="G83" s="22"/>
-      <c r="H83" s="22"/>
-      <c r="I83" s="22"/>
-      <c r="J83" s="22"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="16"/>
+      <c r="I83" s="16"/>
+      <c r="J83" s="16"/>
       <c r="K83" s="3" t="s">
         <v>20</v>
       </c>
@@ -3379,12 +3385,12 @@
         <v>181</v>
       </c>
       <c r="D84" s="2"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="22"/>
-      <c r="G84" s="22"/>
-      <c r="H84" s="22"/>
-      <c r="I84" s="22"/>
-      <c r="J84" s="22"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16"/>
+      <c r="I84" s="16"/>
+      <c r="J84" s="16"/>
       <c r="K84" s="3" t="s">
         <v>182</v>
       </c>
@@ -3397,12 +3403,12 @@
         <v>183</v>
       </c>
       <c r="D85" s="2"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="22"/>
-      <c r="G85" s="22"/>
-      <c r="H85" s="22"/>
-      <c r="I85" s="22"/>
-      <c r="J85" s="22"/>
+      <c r="E85" s="16"/>
+      <c r="F85" s="16"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="16"/>
+      <c r="I85" s="16"/>
+      <c r="J85" s="16"/>
       <c r="K85" s="3" t="s">
         <v>184</v>
       </c>
@@ -3415,12 +3421,12 @@
         <v>185</v>
       </c>
       <c r="D86" s="2"/>
-      <c r="E86" s="22"/>
-      <c r="F86" s="22"/>
-      <c r="G86" s="22"/>
-      <c r="H86" s="22"/>
-      <c r="I86" s="22"/>
-      <c r="J86" s="22"/>
+      <c r="E86" s="16"/>
+      <c r="F86" s="16"/>
+      <c r="G86" s="16"/>
+      <c r="H86" s="16"/>
+      <c r="I86" s="16"/>
+      <c r="J86" s="16"/>
       <c r="K86" s="3" t="s">
         <v>186</v>
       </c>
@@ -3433,12 +3439,12 @@
         <v>187</v>
       </c>
       <c r="D87" s="2"/>
-      <c r="E87" s="22"/>
-      <c r="F87" s="22"/>
-      <c r="G87" s="22"/>
-      <c r="H87" s="22"/>
-      <c r="I87" s="22"/>
-      <c r="J87" s="22"/>
+      <c r="E87" s="16"/>
+      <c r="F87" s="16"/>
+      <c r="G87" s="16"/>
+      <c r="H87" s="16"/>
+      <c r="I87" s="16"/>
+      <c r="J87" s="16"/>
       <c r="K87" s="3" t="s">
         <v>188</v>
       </c>
@@ -3451,12 +3457,12 @@
         <v>189</v>
       </c>
       <c r="D88" s="2"/>
-      <c r="E88" s="22"/>
-      <c r="F88" s="22"/>
-      <c r="G88" s="22"/>
-      <c r="H88" s="22"/>
-      <c r="I88" s="22"/>
-      <c r="J88" s="22"/>
+      <c r="E88" s="16"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="16"/>
+      <c r="H88" s="16"/>
+      <c r="I88" s="16"/>
+      <c r="J88" s="16"/>
       <c r="K88" s="3" t="s">
         <v>190</v>
       </c>
@@ -3469,12 +3475,12 @@
         <v>191</v>
       </c>
       <c r="D89" s="2"/>
-      <c r="E89" s="22"/>
-      <c r="F89" s="22"/>
-      <c r="G89" s="22"/>
-      <c r="H89" s="22"/>
-      <c r="I89" s="22"/>
-      <c r="J89" s="22"/>
+      <c r="E89" s="16"/>
+      <c r="F89" s="16"/>
+      <c r="G89" s="16"/>
+      <c r="H89" s="16"/>
+      <c r="I89" s="16"/>
+      <c r="J89" s="16"/>
       <c r="K89" s="3" t="s">
         <v>192</v>
       </c>
@@ -3487,12 +3493,12 @@
         <v>193</v>
       </c>
       <c r="D90" s="2"/>
-      <c r="E90" s="22"/>
-      <c r="F90" s="22"/>
-      <c r="G90" s="22"/>
-      <c r="H90" s="22"/>
-      <c r="I90" s="22"/>
-      <c r="J90" s="22"/>
+      <c r="E90" s="16"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="16"/>
+      <c r="H90" s="16"/>
+      <c r="I90" s="16"/>
+      <c r="J90" s="16"/>
       <c r="K90" s="3" t="s">
         <v>194</v>
       </c>
@@ -3505,12 +3511,12 @@
         <v>195</v>
       </c>
       <c r="D91" s="2"/>
-      <c r="E91" s="22"/>
-      <c r="F91" s="22"/>
-      <c r="G91" s="22"/>
-      <c r="H91" s="22"/>
-      <c r="I91" s="22"/>
-      <c r="J91" s="22"/>
+      <c r="E91" s="16"/>
+      <c r="F91" s="16"/>
+      <c r="G91" s="16"/>
+      <c r="H91" s="16"/>
+      <c r="I91" s="16"/>
+      <c r="J91" s="16"/>
       <c r="K91" s="3" t="s">
         <v>196</v>
       </c>
@@ -3523,12 +3529,12 @@
         <v>197</v>
       </c>
       <c r="D92" s="2"/>
-      <c r="E92" s="22"/>
-      <c r="F92" s="22"/>
-      <c r="G92" s="22"/>
-      <c r="H92" s="22"/>
-      <c r="I92" s="22"/>
-      <c r="J92" s="22"/>
+      <c r="E92" s="16"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="16"/>
+      <c r="H92" s="16"/>
+      <c r="I92" s="16"/>
+      <c r="J92" s="16"/>
       <c r="K92" s="3" t="s">
         <v>198</v>
       </c>
@@ -3541,12 +3547,12 @@
         <v>199</v>
       </c>
       <c r="D93" s="2"/>
-      <c r="E93" s="22"/>
-      <c r="F93" s="22"/>
-      <c r="G93" s="22"/>
-      <c r="H93" s="22"/>
-      <c r="I93" s="22"/>
-      <c r="J93" s="22"/>
+      <c r="E93" s="16"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="16"/>
+      <c r="H93" s="16"/>
+      <c r="I93" s="16"/>
+      <c r="J93" s="16"/>
       <c r="K93" s="3" t="s">
         <v>200</v>
       </c>
@@ -3559,12 +3565,12 @@
         <v>201</v>
       </c>
       <c r="D94" s="2"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="22"/>
-      <c r="G94" s="22"/>
-      <c r="H94" s="22"/>
-      <c r="I94" s="22"/>
-      <c r="J94" s="22"/>
+      <c r="E94" s="16"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="16"/>
+      <c r="H94" s="16"/>
+      <c r="I94" s="16"/>
+      <c r="J94" s="16"/>
       <c r="K94" s="3" t="s">
         <v>202</v>
       </c>
@@ -3577,12 +3583,12 @@
         <v>203</v>
       </c>
       <c r="D95" s="2"/>
-      <c r="E95" s="22"/>
-      <c r="F95" s="22"/>
-      <c r="G95" s="22"/>
-      <c r="H95" s="22"/>
-      <c r="I95" s="22"/>
-      <c r="J95" s="22"/>
+      <c r="E95" s="16"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="16"/>
+      <c r="H95" s="16"/>
+      <c r="I95" s="16"/>
+      <c r="J95" s="16"/>
       <c r="K95" s="3" t="s">
         <v>204</v>
       </c>
@@ -3595,12 +3601,12 @@
         <v>205</v>
       </c>
       <c r="D96" s="2"/>
-      <c r="E96" s="22"/>
-      <c r="F96" s="22"/>
-      <c r="G96" s="22"/>
-      <c r="H96" s="22"/>
-      <c r="I96" s="22"/>
-      <c r="J96" s="22"/>
+      <c r="E96" s="16"/>
+      <c r="F96" s="16"/>
+      <c r="G96" s="16"/>
+      <c r="H96" s="16"/>
+      <c r="I96" s="16"/>
+      <c r="J96" s="16"/>
       <c r="K96" s="3" t="s">
         <v>206</v>
       </c>
@@ -3613,12 +3619,12 @@
         <v>207</v>
       </c>
       <c r="D97" s="2"/>
-      <c r="E97" s="22"/>
-      <c r="F97" s="22"/>
-      <c r="G97" s="22"/>
-      <c r="H97" s="22"/>
-      <c r="I97" s="22"/>
-      <c r="J97" s="22"/>
+      <c r="E97" s="16"/>
+      <c r="F97" s="16"/>
+      <c r="G97" s="16"/>
+      <c r="H97" s="16"/>
+      <c r="I97" s="16"/>
+      <c r="J97" s="16"/>
       <c r="K97" s="3" t="s">
         <v>208</v>
       </c>
@@ -3631,12 +3637,12 @@
         <v>209</v>
       </c>
       <c r="D98" s="2"/>
-      <c r="E98" s="22"/>
-      <c r="F98" s="22"/>
-      <c r="G98" s="22"/>
-      <c r="H98" s="22"/>
-      <c r="I98" s="22"/>
-      <c r="J98" s="22"/>
+      <c r="E98" s="16"/>
+      <c r="F98" s="16"/>
+      <c r="G98" s="16"/>
+      <c r="H98" s="16"/>
+      <c r="I98" s="16"/>
+      <c r="J98" s="16"/>
       <c r="K98" s="3" t="s">
         <v>210</v>
       </c>
@@ -3649,12 +3655,12 @@
         <v>211</v>
       </c>
       <c r="D99" s="2"/>
-      <c r="E99" s="22"/>
-      <c r="F99" s="22"/>
-      <c r="G99" s="22"/>
-      <c r="H99" s="22"/>
-      <c r="I99" s="22"/>
-      <c r="J99" s="22"/>
+      <c r="E99" s="16"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="16"/>
+      <c r="H99" s="16"/>
+      <c r="I99" s="16"/>
+      <c r="J99" s="16"/>
       <c r="K99" s="3" t="s">
         <v>212</v>
       </c>
@@ -3667,12 +3673,12 @@
         <v>213</v>
       </c>
       <c r="D100" s="2"/>
-      <c r="E100" s="22"/>
-      <c r="F100" s="22"/>
-      <c r="G100" s="22"/>
-      <c r="H100" s="22"/>
-      <c r="I100" s="22"/>
-      <c r="J100" s="22"/>
+      <c r="E100" s="16"/>
+      <c r="F100" s="16"/>
+      <c r="G100" s="16"/>
+      <c r="H100" s="16"/>
+      <c r="I100" s="16"/>
+      <c r="J100" s="16"/>
       <c r="K100" s="3" t="s">
         <v>214</v>
       </c>
@@ -3685,12 +3691,12 @@
         <v>215</v>
       </c>
       <c r="D101" s="2"/>
-      <c r="E101" s="22"/>
-      <c r="F101" s="22"/>
-      <c r="G101" s="22"/>
-      <c r="H101" s="22"/>
-      <c r="I101" s="22"/>
-      <c r="J101" s="22"/>
+      <c r="E101" s="16"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="16"/>
+      <c r="H101" s="16"/>
+      <c r="I101" s="16"/>
+      <c r="J101" s="16"/>
       <c r="K101" s="3" t="s">
         <v>216</v>
       </c>
@@ -3703,12 +3709,12 @@
         <v>219</v>
       </c>
       <c r="D102" s="2"/>
-      <c r="E102" s="22"/>
-      <c r="F102" s="22"/>
-      <c r="G102" s="22"/>
-      <c r="H102" s="22"/>
-      <c r="I102" s="22"/>
-      <c r="J102" s="22"/>
+      <c r="E102" s="16"/>
+      <c r="F102" s="16"/>
+      <c r="G102" s="16"/>
+      <c r="H102" s="16"/>
+      <c r="I102" s="16"/>
+      <c r="J102" s="16"/>
       <c r="K102" s="3" t="s">
         <v>220</v>
       </c>
@@ -3721,12 +3727,12 @@
         <v>221</v>
       </c>
       <c r="D103" s="2"/>
-      <c r="E103" s="22"/>
-      <c r="F103" s="22"/>
-      <c r="G103" s="22"/>
-      <c r="H103" s="22"/>
-      <c r="I103" s="22"/>
-      <c r="J103" s="22"/>
+      <c r="E103" s="16"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="16"/>
+      <c r="H103" s="16"/>
+      <c r="I103" s="16"/>
+      <c r="J103" s="16"/>
       <c r="K103" s="3" t="s">
         <v>222</v>
       </c>
@@ -3739,12 +3745,12 @@
         <v>223</v>
       </c>
       <c r="D104" s="2"/>
-      <c r="E104" s="22"/>
-      <c r="F104" s="22"/>
-      <c r="G104" s="22"/>
-      <c r="H104" s="22"/>
-      <c r="I104" s="22"/>
-      <c r="J104" s="22"/>
+      <c r="E104" s="16"/>
+      <c r="F104" s="16"/>
+      <c r="G104" s="16"/>
+      <c r="H104" s="16"/>
+      <c r="I104" s="16"/>
+      <c r="J104" s="16"/>
       <c r="K104" s="3" t="s">
         <v>224</v>
       </c>
@@ -3757,12 +3763,12 @@
         <v>225</v>
       </c>
       <c r="D105" s="2"/>
-      <c r="E105" s="22"/>
-      <c r="F105" s="22"/>
-      <c r="G105" s="22"/>
-      <c r="H105" s="22"/>
-      <c r="I105" s="22"/>
-      <c r="J105" s="22"/>
+      <c r="E105" s="16"/>
+      <c r="F105" s="16"/>
+      <c r="G105" s="16"/>
+      <c r="H105" s="16"/>
+      <c r="I105" s="16"/>
+      <c r="J105" s="16"/>
       <c r="K105" s="3" t="s">
         <v>226</v>
       </c>
@@ -3775,12 +3781,12 @@
         <v>227</v>
       </c>
       <c r="D106" s="2"/>
-      <c r="E106" s="22"/>
-      <c r="F106" s="22"/>
-      <c r="G106" s="22"/>
-      <c r="H106" s="22"/>
-      <c r="I106" s="22"/>
-      <c r="J106" s="22"/>
+      <c r="E106" s="16"/>
+      <c r="F106" s="16"/>
+      <c r="G106" s="16"/>
+      <c r="H106" s="16"/>
+      <c r="I106" s="16"/>
+      <c r="J106" s="16"/>
       <c r="K106" s="3" t="s">
         <v>228</v>
       </c>
@@ -3793,12 +3799,12 @@
         <v>229</v>
       </c>
       <c r="D107" s="2"/>
-      <c r="E107" s="22"/>
-      <c r="F107" s="22"/>
-      <c r="G107" s="22"/>
-      <c r="H107" s="22"/>
-      <c r="I107" s="22"/>
-      <c r="J107" s="22"/>
+      <c r="E107" s="16"/>
+      <c r="F107" s="16"/>
+      <c r="G107" s="16"/>
+      <c r="H107" s="16"/>
+      <c r="I107" s="16"/>
+      <c r="J107" s="16"/>
       <c r="K107" s="3" t="s">
         <v>230</v>
       </c>
@@ -3811,12 +3817,12 @@
         <v>231</v>
       </c>
       <c r="D108" s="2"/>
-      <c r="E108" s="22"/>
-      <c r="F108" s="22"/>
-      <c r="G108" s="22"/>
-      <c r="H108" s="22"/>
-      <c r="I108" s="22"/>
-      <c r="J108" s="22"/>
+      <c r="E108" s="16"/>
+      <c r="F108" s="16"/>
+      <c r="G108" s="16"/>
+      <c r="H108" s="16"/>
+      <c r="I108" s="16"/>
+      <c r="J108" s="16"/>
       <c r="K108" s="3" t="s">
         <v>232</v>
       </c>
@@ -3829,12 +3835,12 @@
         <v>233</v>
       </c>
       <c r="D109" s="2"/>
-      <c r="E109" s="22"/>
-      <c r="F109" s="22"/>
-      <c r="G109" s="22"/>
-      <c r="H109" s="22"/>
-      <c r="I109" s="22"/>
-      <c r="J109" s="22"/>
+      <c r="E109" s="16"/>
+      <c r="F109" s="16"/>
+      <c r="G109" s="16"/>
+      <c r="H109" s="16"/>
+      <c r="I109" s="16"/>
+      <c r="J109" s="16"/>
       <c r="K109" s="3" t="s">
         <v>234</v>
       </c>
@@ -3847,12 +3853,12 @@
         <v>235</v>
       </c>
       <c r="D110" s="2"/>
-      <c r="E110" s="22"/>
-      <c r="F110" s="22"/>
-      <c r="G110" s="22"/>
-      <c r="H110" s="22"/>
-      <c r="I110" s="22"/>
-      <c r="J110" s="22"/>
+      <c r="E110" s="16"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="16"/>
+      <c r="H110" s="16"/>
+      <c r="I110" s="16"/>
+      <c r="J110" s="16"/>
       <c r="K110" s="3" t="s">
         <v>236</v>
       </c>
@@ -3865,12 +3871,12 @@
         <v>237</v>
       </c>
       <c r="D111" s="2"/>
-      <c r="E111" s="22"/>
-      <c r="F111" s="22"/>
-      <c r="G111" s="22"/>
-      <c r="H111" s="22"/>
-      <c r="I111" s="22"/>
-      <c r="J111" s="22"/>
+      <c r="E111" s="16"/>
+      <c r="F111" s="16"/>
+      <c r="G111" s="16"/>
+      <c r="H111" s="16"/>
+      <c r="I111" s="16"/>
+      <c r="J111" s="16"/>
       <c r="K111" s="3" t="s">
         <v>238</v>
       </c>
@@ -3883,12 +3889,12 @@
         <v>239</v>
       </c>
       <c r="D112" s="2"/>
-      <c r="E112" s="22"/>
-      <c r="F112" s="22"/>
-      <c r="G112" s="22"/>
-      <c r="H112" s="22"/>
-      <c r="I112" s="22"/>
-      <c r="J112" s="22"/>
+      <c r="E112" s="16"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="16"/>
+      <c r="H112" s="16"/>
+      <c r="I112" s="16"/>
+      <c r="J112" s="16"/>
       <c r="K112" s="3" t="s">
         <v>240</v>
       </c>
@@ -3901,12 +3907,12 @@
         <v>241</v>
       </c>
       <c r="D113" s="2"/>
-      <c r="E113" s="22"/>
-      <c r="F113" s="22"/>
-      <c r="G113" s="22"/>
-      <c r="H113" s="22"/>
-      <c r="I113" s="22"/>
-      <c r="J113" s="22"/>
+      <c r="E113" s="16"/>
+      <c r="F113" s="16"/>
+      <c r="G113" s="16"/>
+      <c r="H113" s="16"/>
+      <c r="I113" s="16"/>
+      <c r="J113" s="16"/>
       <c r="K113" s="3" t="s">
         <v>242</v>
       </c>
@@ -3919,12 +3925,12 @@
         <v>243</v>
       </c>
       <c r="D114" s="2"/>
-      <c r="E114" s="22"/>
-      <c r="F114" s="22"/>
-      <c r="G114" s="22"/>
-      <c r="H114" s="22"/>
-      <c r="I114" s="22"/>
-      <c r="J114" s="22"/>
+      <c r="E114" s="16"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="16"/>
+      <c r="H114" s="16"/>
+      <c r="I114" s="16"/>
+      <c r="J114" s="16"/>
       <c r="K114" s="3" t="s">
         <v>244</v>
       </c>
@@ -3937,12 +3943,12 @@
         <v>245</v>
       </c>
       <c r="D115" s="2"/>
-      <c r="E115" s="22"/>
-      <c r="F115" s="22"/>
-      <c r="G115" s="22"/>
-      <c r="H115" s="22"/>
-      <c r="I115" s="22"/>
-      <c r="J115" s="22"/>
+      <c r="E115" s="16"/>
+      <c r="F115" s="16"/>
+      <c r="G115" s="16"/>
+      <c r="H115" s="16"/>
+      <c r="I115" s="16"/>
+      <c r="J115" s="16"/>
       <c r="K115" s="3" t="s">
         <v>246</v>
       </c>
@@ -3955,12 +3961,12 @@
         <v>142</v>
       </c>
       <c r="D116" s="2"/>
-      <c r="E116" s="22"/>
-      <c r="F116" s="22"/>
-      <c r="G116" s="22"/>
-      <c r="H116" s="22"/>
-      <c r="I116" s="22"/>
-      <c r="J116" s="22"/>
+      <c r="E116" s="16"/>
+      <c r="F116" s="16"/>
+      <c r="G116" s="16"/>
+      <c r="H116" s="16"/>
+      <c r="I116" s="16"/>
+      <c r="J116" s="16"/>
       <c r="K116" s="3" t="s">
         <v>141</v>
       </c>
@@ -3973,12 +3979,12 @@
         <v>247</v>
       </c>
       <c r="D117" s="2"/>
-      <c r="E117" s="22"/>
-      <c r="F117" s="22"/>
-      <c r="G117" s="22"/>
-      <c r="H117" s="22"/>
-      <c r="I117" s="22"/>
-      <c r="J117" s="22"/>
+      <c r="E117" s="16"/>
+      <c r="F117" s="16"/>
+      <c r="G117" s="16"/>
+      <c r="H117" s="16"/>
+      <c r="I117" s="16"/>
+      <c r="J117" s="16"/>
       <c r="K117" s="3" t="s">
         <v>248</v>
       </c>
@@ -3991,12 +3997,12 @@
         <v>249</v>
       </c>
       <c r="D118" s="2"/>
-      <c r="E118" s="22"/>
-      <c r="F118" s="22"/>
-      <c r="G118" s="22"/>
-      <c r="H118" s="22"/>
-      <c r="I118" s="22"/>
-      <c r="J118" s="22"/>
+      <c r="E118" s="16"/>
+      <c r="F118" s="16"/>
+      <c r="G118" s="16"/>
+      <c r="H118" s="16"/>
+      <c r="I118" s="16"/>
+      <c r="J118" s="16"/>
       <c r="K118" s="3" t="s">
         <v>250</v>
       </c>
@@ -4009,12 +4015,12 @@
         <v>251</v>
       </c>
       <c r="D119" s="2"/>
-      <c r="E119" s="22"/>
-      <c r="F119" s="22"/>
-      <c r="G119" s="22"/>
-      <c r="H119" s="22"/>
-      <c r="I119" s="22"/>
-      <c r="J119" s="22"/>
+      <c r="E119" s="16"/>
+      <c r="F119" s="16"/>
+      <c r="G119" s="16"/>
+      <c r="H119" s="16"/>
+      <c r="I119" s="16"/>
+      <c r="J119" s="16"/>
       <c r="K119" s="3" t="s">
         <v>252</v>
       </c>
@@ -4027,12 +4033,12 @@
         <v>253</v>
       </c>
       <c r="D120" s="2"/>
-      <c r="E120" s="22"/>
-      <c r="F120" s="22"/>
-      <c r="G120" s="22"/>
-      <c r="H120" s="22"/>
-      <c r="I120" s="22"/>
-      <c r="J120" s="22"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="16"/>
+      <c r="G120" s="16"/>
+      <c r="H120" s="16"/>
+      <c r="I120" s="16"/>
+      <c r="J120" s="16"/>
       <c r="K120" s="3" t="s">
         <v>254</v>
       </c>
@@ -4045,12 +4051,12 @@
         <v>255</v>
       </c>
       <c r="D121" s="2"/>
-      <c r="E121" s="22"/>
-      <c r="F121" s="22"/>
-      <c r="G121" s="22"/>
-      <c r="H121" s="22"/>
-      <c r="I121" s="22"/>
-      <c r="J121" s="22"/>
+      <c r="E121" s="16"/>
+      <c r="F121" s="16"/>
+      <c r="G121" s="16"/>
+      <c r="H121" s="16"/>
+      <c r="I121" s="16"/>
+      <c r="J121" s="16"/>
       <c r="K121" s="3" t="s">
         <v>256</v>
       </c>
@@ -4063,12 +4069,12 @@
         <v>257</v>
       </c>
       <c r="D122" s="2"/>
-      <c r="E122" s="22"/>
-      <c r="F122" s="22"/>
-      <c r="G122" s="22"/>
-      <c r="H122" s="22"/>
-      <c r="I122" s="22"/>
-      <c r="J122" s="22"/>
+      <c r="E122" s="16"/>
+      <c r="F122" s="16"/>
+      <c r="G122" s="16"/>
+      <c r="H122" s="16"/>
+      <c r="I122" s="16"/>
+      <c r="J122" s="16"/>
       <c r="K122" s="3" t="s">
         <v>258</v>
       </c>
@@ -4081,12 +4087,12 @@
         <v>259</v>
       </c>
       <c r="D123" s="2"/>
-      <c r="E123" s="22"/>
-      <c r="F123" s="22"/>
-      <c r="G123" s="22"/>
-      <c r="H123" s="22"/>
-      <c r="I123" s="22"/>
-      <c r="J123" s="22"/>
+      <c r="E123" s="16"/>
+      <c r="F123" s="16"/>
+      <c r="G123" s="16"/>
+      <c r="H123" s="16"/>
+      <c r="I123" s="16"/>
+      <c r="J123" s="16"/>
       <c r="K123" s="3" t="s">
         <v>260</v>
       </c>
@@ -4099,12 +4105,12 @@
         <v>261</v>
       </c>
       <c r="D124" s="2"/>
-      <c r="E124" s="22"/>
-      <c r="F124" s="22"/>
-      <c r="G124" s="22"/>
-      <c r="H124" s="22"/>
-      <c r="I124" s="22"/>
-      <c r="J124" s="22"/>
+      <c r="E124" s="16"/>
+      <c r="F124" s="16"/>
+      <c r="G124" s="16"/>
+      <c r="H124" s="16"/>
+      <c r="I124" s="16"/>
+      <c r="J124" s="16"/>
       <c r="K124" s="3" t="s">
         <v>262</v>
       </c>
@@ -4117,12 +4123,12 @@
         <v>263</v>
       </c>
       <c r="D125" s="2"/>
-      <c r="E125" s="22"/>
-      <c r="F125" s="22"/>
-      <c r="G125" s="22"/>
-      <c r="H125" s="22"/>
-      <c r="I125" s="22"/>
-      <c r="J125" s="22"/>
+      <c r="E125" s="16"/>
+      <c r="F125" s="16"/>
+      <c r="G125" s="16"/>
+      <c r="H125" s="16"/>
+      <c r="I125" s="16"/>
+      <c r="J125" s="16"/>
       <c r="K125" s="3" t="s">
         <v>264</v>
       </c>
@@ -4135,12 +4141,12 @@
         <v>265</v>
       </c>
       <c r="D126" s="2"/>
-      <c r="E126" s="22"/>
-      <c r="F126" s="22"/>
-      <c r="G126" s="22"/>
-      <c r="H126" s="22"/>
-      <c r="I126" s="22"/>
-      <c r="J126" s="22"/>
+      <c r="E126" s="16"/>
+      <c r="F126" s="16"/>
+      <c r="G126" s="16"/>
+      <c r="H126" s="16"/>
+      <c r="I126" s="16"/>
+      <c r="J126" s="16"/>
       <c r="K126" s="3" t="s">
         <v>266</v>
       </c>
@@ -4153,12 +4159,12 @@
         <v>267</v>
       </c>
       <c r="D127" s="2"/>
-      <c r="E127" s="22"/>
-      <c r="F127" s="22"/>
-      <c r="G127" s="22"/>
-      <c r="H127" s="22"/>
-      <c r="I127" s="22"/>
-      <c r="J127" s="22"/>
+      <c r="E127" s="16"/>
+      <c r="F127" s="16"/>
+      <c r="G127" s="16"/>
+      <c r="H127" s="16"/>
+      <c r="I127" s="16"/>
+      <c r="J127" s="16"/>
       <c r="K127" s="3" t="s">
         <v>268</v>
       </c>
@@ -4171,12 +4177,12 @@
         <v>269</v>
       </c>
       <c r="D128" s="2"/>
-      <c r="E128" s="22"/>
-      <c r="F128" s="22"/>
-      <c r="G128" s="22"/>
-      <c r="H128" s="22"/>
-      <c r="I128" s="22"/>
-      <c r="J128" s="22"/>
+      <c r="E128" s="16"/>
+      <c r="F128" s="16"/>
+      <c r="G128" s="16"/>
+      <c r="H128" s="16"/>
+      <c r="I128" s="16"/>
+      <c r="J128" s="16"/>
       <c r="K128" s="3" t="s">
         <v>270</v>
       </c>
@@ -4189,12 +4195,12 @@
         <v>271</v>
       </c>
       <c r="D129" s="2"/>
-      <c r="E129" s="22"/>
-      <c r="F129" s="22"/>
-      <c r="G129" s="22"/>
-      <c r="H129" s="22"/>
-      <c r="I129" s="22"/>
-      <c r="J129" s="22"/>
+      <c r="E129" s="16"/>
+      <c r="F129" s="16"/>
+      <c r="G129" s="16"/>
+      <c r="H129" s="16"/>
+      <c r="I129" s="16"/>
+      <c r="J129" s="16"/>
       <c r="K129" s="3" t="s">
         <v>272</v>
       </c>
@@ -4207,12 +4213,12 @@
         <v>273</v>
       </c>
       <c r="D130" s="2"/>
-      <c r="E130" s="22"/>
-      <c r="F130" s="22"/>
-      <c r="G130" s="22"/>
-      <c r="H130" s="22"/>
-      <c r="I130" s="22"/>
-      <c r="J130" s="22"/>
+      <c r="E130" s="16"/>
+      <c r="F130" s="16"/>
+      <c r="G130" s="16"/>
+      <c r="H130" s="16"/>
+      <c r="I130" s="16"/>
+      <c r="J130" s="16"/>
       <c r="K130" s="3" t="s">
         <v>274</v>
       </c>
@@ -4225,12 +4231,12 @@
         <v>275</v>
       </c>
       <c r="D131" s="2"/>
-      <c r="E131" s="22"/>
-      <c r="F131" s="22"/>
-      <c r="G131" s="22"/>
-      <c r="H131" s="22"/>
-      <c r="I131" s="22"/>
-      <c r="J131" s="22"/>
+      <c r="E131" s="16"/>
+      <c r="F131" s="16"/>
+      <c r="G131" s="16"/>
+      <c r="H131" s="16"/>
+      <c r="I131" s="16"/>
+      <c r="J131" s="16"/>
       <c r="K131" s="3" t="s">
         <v>276</v>
       </c>
@@ -4243,12 +4249,12 @@
         <v>277</v>
       </c>
       <c r="D132" s="2"/>
-      <c r="E132" s="22"/>
-      <c r="F132" s="22"/>
-      <c r="G132" s="22"/>
-      <c r="H132" s="22"/>
-      <c r="I132" s="22"/>
-      <c r="J132" s="22"/>
+      <c r="E132" s="16"/>
+      <c r="F132" s="16"/>
+      <c r="G132" s="16"/>
+      <c r="H132" s="16"/>
+      <c r="I132" s="16"/>
+      <c r="J132" s="16"/>
       <c r="K132" s="3" t="s">
         <v>278</v>
       </c>
@@ -4261,12 +4267,12 @@
         <v>279</v>
       </c>
       <c r="D133" s="2"/>
-      <c r="E133" s="22"/>
-      <c r="F133" s="22"/>
-      <c r="G133" s="22"/>
-      <c r="H133" s="22"/>
-      <c r="I133" s="22"/>
-      <c r="J133" s="22"/>
+      <c r="E133" s="16"/>
+      <c r="F133" s="16"/>
+      <c r="G133" s="16"/>
+      <c r="H133" s="16"/>
+      <c r="I133" s="16"/>
+      <c r="J133" s="16"/>
       <c r="K133" s="3" t="s">
         <v>280</v>
       </c>
@@ -4279,12 +4285,12 @@
         <v>281</v>
       </c>
       <c r="D134" s="2"/>
-      <c r="E134" s="22"/>
-      <c r="F134" s="22"/>
-      <c r="G134" s="22"/>
-      <c r="H134" s="22"/>
-      <c r="I134" s="22"/>
-      <c r="J134" s="22"/>
+      <c r="E134" s="16"/>
+      <c r="F134" s="16"/>
+      <c r="G134" s="16"/>
+      <c r="H134" s="16"/>
+      <c r="I134" s="16"/>
+      <c r="J134" s="16"/>
       <c r="K134" s="3" t="s">
         <v>282</v>
       </c>
@@ -4297,12 +4303,12 @@
         <v>283</v>
       </c>
       <c r="D135" s="2"/>
-      <c r="E135" s="22"/>
-      <c r="F135" s="22"/>
-      <c r="G135" s="22"/>
-      <c r="H135" s="22"/>
-      <c r="I135" s="22"/>
-      <c r="J135" s="22"/>
+      <c r="E135" s="16"/>
+      <c r="F135" s="16"/>
+      <c r="G135" s="16"/>
+      <c r="H135" s="16"/>
+      <c r="I135" s="16"/>
+      <c r="J135" s="16"/>
       <c r="K135" s="3" t="s">
         <v>284</v>
       </c>
@@ -4315,12 +4321,12 @@
         <v>285</v>
       </c>
       <c r="D136" s="2"/>
-      <c r="E136" s="22"/>
-      <c r="F136" s="22"/>
-      <c r="G136" s="22"/>
-      <c r="H136" s="22"/>
-      <c r="I136" s="22"/>
-      <c r="J136" s="22"/>
+      <c r="E136" s="16"/>
+      <c r="F136" s="16"/>
+      <c r="G136" s="16"/>
+      <c r="H136" s="16"/>
+      <c r="I136" s="16"/>
+      <c r="J136" s="16"/>
       <c r="K136" s="3" t="s">
         <v>286</v>
       </c>
@@ -4333,12 +4339,12 @@
         <v>287</v>
       </c>
       <c r="D137" s="2"/>
-      <c r="E137" s="22"/>
-      <c r="F137" s="22"/>
-      <c r="G137" s="22"/>
-      <c r="H137" s="22"/>
-      <c r="I137" s="22"/>
-      <c r="J137" s="22"/>
+      <c r="E137" s="16"/>
+      <c r="F137" s="16"/>
+      <c r="G137" s="16"/>
+      <c r="H137" s="16"/>
+      <c r="I137" s="16"/>
+      <c r="J137" s="16"/>
       <c r="K137" s="3" t="s">
         <v>288</v>
       </c>
@@ -4351,12 +4357,12 @@
         <v>289</v>
       </c>
       <c r="D138" s="2"/>
-      <c r="E138" s="22"/>
-      <c r="F138" s="22"/>
-      <c r="G138" s="22"/>
-      <c r="H138" s="22"/>
-      <c r="I138" s="22"/>
-      <c r="J138" s="22"/>
+      <c r="E138" s="16"/>
+      <c r="F138" s="16"/>
+      <c r="G138" s="16"/>
+      <c r="H138" s="16"/>
+      <c r="I138" s="16"/>
+      <c r="J138" s="16"/>
       <c r="K138" s="3" t="s">
         <v>290</v>
       </c>
@@ -4369,12 +4375,12 @@
         <v>291</v>
       </c>
       <c r="D139" s="2"/>
-      <c r="E139" s="22"/>
-      <c r="F139" s="22"/>
-      <c r="G139" s="22"/>
-      <c r="H139" s="22"/>
-      <c r="I139" s="22"/>
-      <c r="J139" s="22"/>
+      <c r="E139" s="16"/>
+      <c r="F139" s="16"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="16"/>
+      <c r="I139" s="16"/>
+      <c r="J139" s="16"/>
       <c r="K139" s="3" t="s">
         <v>292</v>
       </c>
@@ -4383,12 +4389,12 @@
       <c r="B140" s="8"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
-      <c r="E140" s="22"/>
-      <c r="F140" s="22"/>
-      <c r="G140" s="22"/>
-      <c r="H140" s="22"/>
-      <c r="I140" s="22"/>
-      <c r="J140" s="22"/>
+      <c r="E140" s="16"/>
+      <c r="F140" s="16"/>
+      <c r="G140" s="16"/>
+      <c r="H140" s="16"/>
+      <c r="I140" s="16"/>
+      <c r="J140" s="16"/>
       <c r="K140" s="2"/>
     </row>
     <row r="141" spans="2:11">
@@ -4577,13 +4583,13 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">

</xml_diff>